<commit_message>
Minor changes to CalcTakeOff and CalcLanding. More work on thesis in DOCS/Theses/Trifari. Minor changes in JPAD_INPUT.xls
</commit_message>
<xml_diff>
--- a/DOCS/InputFile/JPAD_INPUT.xlsx
+++ b/DOCS/InputFile/JPAD_INPUT.xlsx
@@ -411,7 +411,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="237">
   <si>
     <t>JPAD INPUT DATA</t>
   </si>
@@ -1104,6 +1104,24 @@
   </si>
   <si>
     <t>Eta Out Slat</t>
+  </si>
+  <si>
+    <t>Ksfc</t>
+  </si>
+  <si>
+    <t>Kcruise</t>
+  </si>
+  <si>
+    <t>KTakeOff</t>
+  </si>
+  <si>
+    <t>Kdescent</t>
+  </si>
+  <si>
+    <t>Kclimb</t>
+  </si>
+  <si>
+    <t>Kcontinous</t>
   </si>
 </sst>
 </file>
@@ -1482,8 +1500,123 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1511,9 +1644,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1523,118 +1653,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1942,69 +1961,69 @@
   <dimension ref="A1:AI147"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Z15" sqref="Z15"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.77734375" style="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.77734375" style="29" customWidth="1"/>
-    <col min="3" max="3" width="17" style="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.44140625" style="29" customWidth="1"/>
-    <col min="5" max="5" width="26.5546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.109375" style="29" customWidth="1"/>
-    <col min="7" max="7" width="51.44140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.44140625" style="29" customWidth="1"/>
-    <col min="9" max="9" width="46.109375" style="29" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.109375" style="29" customWidth="1"/>
-    <col min="11" max="11" width="41.44140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.88671875" style="29"/>
-    <col min="13" max="13" width="37.6640625" style="29" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" style="29"/>
-    <col min="15" max="15" width="41.44140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.88671875" style="29"/>
-    <col min="17" max="17" width="17" style="29" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.21875" style="29" customWidth="1"/>
-    <col min="19" max="19" width="49.44140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.44140625" style="29" customWidth="1"/>
-    <col min="21" max="21" width="49.44140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.44140625" style="29" customWidth="1"/>
-    <col min="23" max="23" width="49.44140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.88671875" style="29" customWidth="1"/>
-    <col min="25" max="25" width="17" style="29" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.77734375" style="29" customWidth="1"/>
-    <col min="27" max="35" width="8.88671875" style="29"/>
+    <col min="1" max="1" width="44.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.77734375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="17" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.44140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="26.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="51.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.44140625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="46.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.109375" style="6" customWidth="1"/>
+    <col min="11" max="11" width="41.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" style="6"/>
+    <col min="13" max="13" width="37.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.88671875" style="6"/>
+    <col min="15" max="15" width="41.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.88671875" style="6"/>
+    <col min="17" max="17" width="17" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.21875" style="6" customWidth="1"/>
+    <col min="19" max="19" width="49.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.44140625" style="6" customWidth="1"/>
+    <col min="21" max="21" width="49.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.44140625" style="6" customWidth="1"/>
+    <col min="23" max="23" width="49.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.88671875" style="6" customWidth="1"/>
+    <col min="25" max="25" width="17" style="6" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.77734375" style="6" customWidth="1"/>
+    <col min="27" max="35" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="3"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="58"/>
       <c r="AA1"/>
       <c r="AB1"/>
       <c r="AC1"/>
@@ -2016,32 +2035,32 @@
       <c r="AI1"/>
     </row>
     <row r="2" spans="1:35" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5"/>
-      <c r="Z2" s="6"/>
+      <c r="A2" s="59"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="60"/>
+      <c r="S2" s="60"/>
+      <c r="T2" s="60"/>
+      <c r="U2" s="60"/>
+      <c r="V2" s="60"/>
+      <c r="W2" s="60"/>
+      <c r="X2" s="60"/>
+      <c r="Y2" s="60"/>
+      <c r="Z2" s="61"/>
       <c r="AA2"/>
       <c r="AB2"/>
       <c r="AC2"/>
@@ -2053,32 +2072,32 @@
       <c r="AI2"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="9"/>
+      <c r="A3" s="62"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="63"/>
+      <c r="N3" s="63"/>
+      <c r="O3" s="63"/>
+      <c r="P3" s="63"/>
+      <c r="Q3" s="63"/>
+      <c r="R3" s="63"/>
+      <c r="S3" s="63"/>
+      <c r="T3" s="63"/>
+      <c r="U3" s="63"/>
+      <c r="V3" s="63"/>
+      <c r="W3" s="63"/>
+      <c r="X3" s="63"/>
+      <c r="Y3" s="63"/>
+      <c r="Z3" s="64"/>
       <c r="AA3"/>
       <c r="AB3"/>
       <c r="AC3"/>
@@ -2090,34 +2109,34 @@
       <c r="AI3"/>
     </row>
     <row r="4" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12"/>
-      <c r="U4" s="12"/>
-      <c r="V4" s="12"/>
-      <c r="W4" s="12"/>
-      <c r="X4" s="12"/>
-      <c r="Y4" s="12"/>
-      <c r="Z4" s="13"/>
+      <c r="B4" s="66"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="66"/>
+      <c r="M4" s="66"/>
+      <c r="N4" s="66"/>
+      <c r="O4" s="66"/>
+      <c r="P4" s="66"/>
+      <c r="Q4" s="66"/>
+      <c r="R4" s="66"/>
+      <c r="S4" s="66"/>
+      <c r="T4" s="66"/>
+      <c r="U4" s="66"/>
+      <c r="V4" s="66"/>
+      <c r="W4" s="66"/>
+      <c r="X4" s="66"/>
+      <c r="Y4" s="66"/>
+      <c r="Z4" s="67"/>
       <c r="AA4"/>
       <c r="AB4"/>
       <c r="AC4"/>
@@ -2129,34 +2148,34 @@
       <c r="AI4"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="57"/>
-      <c r="I5" s="57"/>
-      <c r="J5" s="57"/>
-      <c r="K5" s="57"/>
-      <c r="L5" s="57"/>
-      <c r="M5" s="57"/>
-      <c r="N5" s="57"/>
-      <c r="O5" s="57"/>
-      <c r="P5" s="57"/>
-      <c r="Q5" s="57"/>
-      <c r="R5" s="57"/>
-      <c r="S5" s="57"/>
-      <c r="T5" s="57"/>
-      <c r="U5" s="57"/>
-      <c r="V5" s="57"/>
-      <c r="W5" s="57"/>
-      <c r="X5" s="57"/>
-      <c r="Y5" s="57"/>
-      <c r="Z5" s="58"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="51"/>
+      <c r="N5" s="51"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="51"/>
+      <c r="R5" s="51"/>
+      <c r="S5" s="51"/>
+      <c r="T5" s="51"/>
+      <c r="U5" s="51"/>
+      <c r="V5" s="51"/>
+      <c r="W5" s="51"/>
+      <c r="X5" s="51"/>
+      <c r="Y5" s="51"/>
+      <c r="Z5" s="52"/>
       <c r="AA5"/>
       <c r="AB5"/>
       <c r="AC5"/>
@@ -2168,34 +2187,34 @@
       <c r="AI5"/>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="60"/>
-      <c r="L6" s="60"/>
-      <c r="M6" s="60"/>
-      <c r="N6" s="60"/>
-      <c r="O6" s="60"/>
-      <c r="P6" s="60"/>
-      <c r="Q6" s="60"/>
-      <c r="R6" s="60"/>
-      <c r="S6" s="60"/>
-      <c r="T6" s="60"/>
-      <c r="U6" s="60"/>
-      <c r="V6" s="60"/>
-      <c r="W6" s="60"/>
-      <c r="X6" s="60"/>
-      <c r="Y6" s="60"/>
-      <c r="Z6" s="61"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="54"/>
+      <c r="N6" s="54"/>
+      <c r="O6" s="54"/>
+      <c r="P6" s="54"/>
+      <c r="Q6" s="54"/>
+      <c r="R6" s="54"/>
+      <c r="S6" s="54"/>
+      <c r="T6" s="54"/>
+      <c r="U6" s="54"/>
+      <c r="V6" s="54"/>
+      <c r="W6" s="54"/>
+      <c r="X6" s="54"/>
+      <c r="Y6" s="54"/>
+      <c r="Z6" s="55"/>
       <c r="AA6"/>
       <c r="AB6"/>
       <c r="AC6"/>
@@ -2207,34 +2226,34 @@
       <c r="AI6"/>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="60"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="60"/>
-      <c r="L7" s="60"/>
-      <c r="M7" s="60"/>
-      <c r="N7" s="60"/>
-      <c r="O7" s="60"/>
-      <c r="P7" s="60"/>
-      <c r="Q7" s="60"/>
-      <c r="R7" s="60"/>
-      <c r="S7" s="60"/>
-      <c r="T7" s="60"/>
-      <c r="U7" s="60"/>
-      <c r="V7" s="60"/>
-      <c r="W7" s="60"/>
-      <c r="X7" s="60"/>
-      <c r="Y7" s="60"/>
-      <c r="Z7" s="61"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="54"/>
+      <c r="M7" s="54"/>
+      <c r="N7" s="54"/>
+      <c r="O7" s="54"/>
+      <c r="P7" s="54"/>
+      <c r="Q7" s="54"/>
+      <c r="R7" s="54"/>
+      <c r="S7" s="54"/>
+      <c r="T7" s="54"/>
+      <c r="U7" s="54"/>
+      <c r="V7" s="54"/>
+      <c r="W7" s="54"/>
+      <c r="X7" s="54"/>
+      <c r="Y7" s="54"/>
+      <c r="Z7" s="55"/>
       <c r="AA7"/>
       <c r="AB7"/>
       <c r="AC7"/>
@@ -2246,34 +2265,34 @@
       <c r="AI7"/>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="60"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="60"/>
-      <c r="L8" s="60"/>
-      <c r="M8" s="60"/>
-      <c r="N8" s="60"/>
-      <c r="O8" s="60"/>
-      <c r="P8" s="60"/>
-      <c r="Q8" s="60"/>
-      <c r="R8" s="60"/>
-      <c r="S8" s="60"/>
-      <c r="T8" s="60"/>
-      <c r="U8" s="60"/>
-      <c r="V8" s="60"/>
-      <c r="W8" s="60"/>
-      <c r="X8" s="60"/>
-      <c r="Y8" s="60"/>
-      <c r="Z8" s="61"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="54"/>
+      <c r="M8" s="54"/>
+      <c r="N8" s="54"/>
+      <c r="O8" s="54"/>
+      <c r="P8" s="54"/>
+      <c r="Q8" s="54"/>
+      <c r="R8" s="54"/>
+      <c r="S8" s="54"/>
+      <c r="T8" s="54"/>
+      <c r="U8" s="54"/>
+      <c r="V8" s="54"/>
+      <c r="W8" s="54"/>
+      <c r="X8" s="54"/>
+      <c r="Y8" s="54"/>
+      <c r="Z8" s="55"/>
       <c r="AA8"/>
       <c r="AB8"/>
       <c r="AC8"/>
@@ -2285,34 +2304,34 @@
       <c r="AI8"/>
     </row>
     <row r="9" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="59" t="s">
+      <c r="A9" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="60"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="60"/>
-      <c r="L9" s="60"/>
-      <c r="M9" s="60"/>
-      <c r="N9" s="60"/>
-      <c r="O9" s="60"/>
-      <c r="P9" s="60"/>
-      <c r="Q9" s="60"/>
-      <c r="R9" s="60"/>
-      <c r="S9" s="60"/>
-      <c r="T9" s="60"/>
-      <c r="U9" s="60"/>
-      <c r="V9" s="60"/>
-      <c r="W9" s="60"/>
-      <c r="X9" s="60"/>
-      <c r="Y9" s="60"/>
-      <c r="Z9" s="61"/>
+      <c r="B9" s="54"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="54"/>
+      <c r="M9" s="54"/>
+      <c r="N9" s="54"/>
+      <c r="O9" s="54"/>
+      <c r="P9" s="54"/>
+      <c r="Q9" s="54"/>
+      <c r="R9" s="54"/>
+      <c r="S9" s="54"/>
+      <c r="T9" s="54"/>
+      <c r="U9" s="54"/>
+      <c r="V9" s="54"/>
+      <c r="W9" s="54"/>
+      <c r="X9" s="54"/>
+      <c r="Y9" s="54"/>
+      <c r="Z9" s="55"/>
       <c r="AA9"/>
       <c r="AB9"/>
       <c r="AC9"/>
@@ -2324,34 +2343,34 @@
       <c r="AI9"/>
     </row>
     <row r="10" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="12"/>
-      <c r="S10" s="12"/>
-      <c r="T10" s="12"/>
-      <c r="U10" s="12"/>
-      <c r="V10" s="12"/>
-      <c r="W10" s="12"/>
-      <c r="X10" s="12"/>
-      <c r="Y10" s="12"/>
-      <c r="Z10" s="13"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="66"/>
+      <c r="J10" s="66"/>
+      <c r="K10" s="66"/>
+      <c r="L10" s="66"/>
+      <c r="M10" s="66"/>
+      <c r="N10" s="66"/>
+      <c r="O10" s="66"/>
+      <c r="P10" s="66"/>
+      <c r="Q10" s="66"/>
+      <c r="R10" s="66"/>
+      <c r="S10" s="66"/>
+      <c r="T10" s="66"/>
+      <c r="U10" s="66"/>
+      <c r="V10" s="66"/>
+      <c r="W10" s="66"/>
+      <c r="X10" s="66"/>
+      <c r="Y10" s="66"/>
+      <c r="Z10" s="67"/>
       <c r="AA10"/>
       <c r="AB10"/>
       <c r="AC10"/>
@@ -2362,89 +2381,89 @@
       <c r="AH10"/>
       <c r="AI10"/>
     </row>
-    <row r="11" spans="1:35" s="36" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="42" t="s">
+    <row r="11" spans="1:35" s="13" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="39"/>
-      <c r="L11" s="39"/>
-      <c r="M11" s="39"/>
-      <c r="N11" s="39"/>
-      <c r="O11" s="39"/>
-      <c r="P11" s="39"/>
-      <c r="Q11" s="39"/>
-      <c r="R11" s="39"/>
-      <c r="S11" s="39"/>
-      <c r="T11" s="39"/>
-      <c r="U11" s="39"/>
-      <c r="V11" s="39"/>
-      <c r="W11" s="39"/>
-      <c r="X11" s="39"/>
-      <c r="Y11" s="39"/>
-      <c r="Z11" s="43"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="48"/>
+      <c r="L11" s="48"/>
+      <c r="M11" s="48"/>
+      <c r="N11" s="48"/>
+      <c r="O11" s="48"/>
+      <c r="P11" s="48"/>
+      <c r="Q11" s="48"/>
+      <c r="R11" s="48"/>
+      <c r="S11" s="48"/>
+      <c r="T11" s="48"/>
+      <c r="U11" s="48"/>
+      <c r="V11" s="48"/>
+      <c r="W11" s="48"/>
+      <c r="X11" s="48"/>
+      <c r="Y11" s="48"/>
+      <c r="Z11" s="49"/>
     </row>
     <row r="12" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="22" t="s">
+      <c r="B12" s="36"/>
+      <c r="C12" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="22" t="s">
+      <c r="D12" s="36"/>
+      <c r="E12" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="23"/>
-      <c r="G12" s="22" t="s">
+      <c r="F12" s="36"/>
+      <c r="G12" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="23"/>
-      <c r="I12" s="22" t="s">
+      <c r="H12" s="36"/>
+      <c r="I12" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="J12" s="23"/>
-      <c r="K12" s="22" t="s">
+      <c r="J12" s="36"/>
+      <c r="K12" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="L12" s="23"/>
-      <c r="M12" s="22" t="s">
+      <c r="L12" s="36"/>
+      <c r="M12" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="N12" s="23"/>
-      <c r="O12" s="22" t="s">
+      <c r="N12" s="36"/>
+      <c r="O12" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="22" t="s">
+      <c r="P12" s="36"/>
+      <c r="Q12" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="R12" s="23"/>
-      <c r="S12" s="22" t="s">
+      <c r="R12" s="36"/>
+      <c r="S12" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="T12" s="23"/>
-      <c r="U12" s="22" t="s">
+      <c r="T12" s="36"/>
+      <c r="U12" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="V12" s="23"/>
-      <c r="W12" s="22" t="s">
+      <c r="V12" s="36"/>
+      <c r="W12" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="X12" s="23"/>
-      <c r="Y12" s="22" t="s">
+      <c r="X12" s="36"/>
+      <c r="Y12" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="Z12" s="23"/>
+      <c r="Z12" s="36"/>
       <c r="AA12"/>
       <c r="AB12"/>
       <c r="AC12"/>
@@ -2456,58 +2475,58 @@
       <c r="AI12"/>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="31" t="s">
+      <c r="B13" s="2"/>
+      <c r="C13" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="28"/>
-      <c r="E13" s="31" t="s">
+      <c r="D13" s="5"/>
+      <c r="E13" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="31" t="s">
+      <c r="F13" s="2"/>
+      <c r="G13" s="68" t="s">
         <v>76</v>
       </c>
-      <c r="H13" s="28"/>
-      <c r="I13" s="44" t="s">
+      <c r="H13" s="5"/>
+      <c r="I13" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="J13" s="28"/>
-      <c r="K13" s="24" t="s">
+      <c r="J13" s="5"/>
+      <c r="K13" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="L13" s="45"/>
-      <c r="M13" s="24" t="s">
+      <c r="L13" s="16"/>
+      <c r="M13" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="N13" s="45"/>
-      <c r="O13" s="24" t="s">
+      <c r="N13" s="16"/>
+      <c r="O13" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="P13" s="45"/>
-      <c r="Q13" s="31" t="s">
+      <c r="P13" s="16"/>
+      <c r="Q13" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="R13" s="28"/>
-      <c r="S13" s="31" t="s">
+      <c r="R13" s="5"/>
+      <c r="S13" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="T13" s="25"/>
-      <c r="U13" s="31" t="s">
+      <c r="T13" s="2"/>
+      <c r="U13" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="V13" s="25"/>
-      <c r="W13" s="31" t="s">
+      <c r="V13" s="2"/>
+      <c r="W13" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="X13" s="25"/>
-      <c r="Y13" s="31" t="s">
+      <c r="X13" s="2"/>
+      <c r="Y13" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="Z13" s="25"/>
+      <c r="Z13" s="2"/>
       <c r="AA13"/>
       <c r="AB13"/>
       <c r="AC13"/>
@@ -2519,54 +2538,55 @@
       <c r="AI13"/>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="32" t="s">
+      <c r="B14" s="3"/>
+      <c r="C14" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="32" t="s">
+      <c r="E14" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="G14" s="32" t="s">
+      <c r="F14" s="3"/>
+      <c r="G14" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="H14" s="62"/>
-      <c r="I14" s="52" t="s">
+      <c r="H14" s="20"/>
+      <c r="I14" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="K14" s="32" t="s">
+      <c r="K14" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="L14" s="40"/>
-      <c r="M14" s="32" t="s">
+      <c r="L14" s="14"/>
+      <c r="M14" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="N14" s="26"/>
-      <c r="O14" s="32" t="s">
+      <c r="N14" s="3"/>
+      <c r="O14" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="P14" s="26"/>
-      <c r="Q14" s="32" t="s">
+      <c r="P14" s="3"/>
+      <c r="Q14" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="S14" s="32" t="s">
+      <c r="S14" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="T14" s="26"/>
-      <c r="U14" s="32" t="s">
+      <c r="T14" s="3"/>
+      <c r="U14" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="V14" s="26"/>
-      <c r="W14" s="32" t="s">
+      <c r="V14" s="3"/>
+      <c r="W14" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="X14" s="26"/>
-      <c r="Y14" s="32" t="s">
+      <c r="X14" s="3"/>
+      <c r="Y14" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="Z14" s="26"/>
+      <c r="Z14" s="3"/>
       <c r="AA14"/>
       <c r="AB14"/>
       <c r="AC14"/>
@@ -2578,53 +2598,54 @@
       <c r="AI14"/>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="32" t="s">
+      <c r="B15" s="3"/>
+      <c r="C15" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="32" t="s">
+      <c r="E15" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G15" s="32" t="s">
+      <c r="F15" s="3"/>
+      <c r="G15" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="I15" s="52" t="s">
+      <c r="I15" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="K15" s="32" t="s">
+      <c r="K15" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="L15" s="26"/>
-      <c r="M15" s="34" t="s">
+      <c r="L15" s="3"/>
+      <c r="M15" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="N15" s="26"/>
-      <c r="O15" s="34" t="s">
+      <c r="N15" s="3"/>
+      <c r="O15" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="P15" s="26"/>
-      <c r="Q15" s="32" t="s">
+      <c r="P15" s="3"/>
+      <c r="Q15" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="S15" s="32" t="s">
+      <c r="S15" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="T15" s="26"/>
-      <c r="U15" s="32" t="s">
+      <c r="T15" s="3"/>
+      <c r="U15" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="V15" s="26"/>
-      <c r="W15" s="32" t="s">
+      <c r="V15" s="3"/>
+      <c r="W15" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="X15" s="26"/>
-      <c r="Y15" s="32" t="s">
+      <c r="X15" s="3"/>
+      <c r="Y15" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="Z15" s="26"/>
+      <c r="Z15" s="3"/>
       <c r="AA15"/>
       <c r="AB15"/>
       <c r="AC15"/>
@@ -2636,53 +2657,54 @@
       <c r="AI15"/>
     </row>
     <row r="16" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="32" t="s">
+      <c r="B16" s="3"/>
+      <c r="C16" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="E16" s="32" t="s">
+      <c r="E16" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G16" s="32" t="s">
+      <c r="F16" s="3"/>
+      <c r="G16" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="I16" s="52" t="s">
+      <c r="I16" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="K16" s="32" t="s">
+      <c r="K16" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="L16" s="26"/>
-      <c r="M16" s="34" t="s">
+      <c r="L16" s="3"/>
+      <c r="M16" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="N16" s="26"/>
-      <c r="O16" s="34" t="s">
+      <c r="N16" s="3"/>
+      <c r="O16" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="P16" s="26"/>
-      <c r="Q16" s="32" t="s">
+      <c r="P16" s="3"/>
+      <c r="Q16" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="S16" s="32" t="s">
+      <c r="S16" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="T16" s="26"/>
-      <c r="U16" s="32" t="s">
+      <c r="T16" s="3"/>
+      <c r="U16" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="V16" s="26"/>
-      <c r="W16" s="32" t="s">
+      <c r="V16" s="3"/>
+      <c r="W16" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="X16" s="26"/>
-      <c r="Y16" s="33" t="s">
+      <c r="X16" s="3"/>
+      <c r="Y16" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="Z16" s="27"/>
+      <c r="Z16" s="4"/>
       <c r="AA16"/>
       <c r="AB16"/>
       <c r="AC16"/>
@@ -2694,50 +2716,51 @@
       <c r="AI16"/>
     </row>
     <row r="17" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="32" t="s">
+      <c r="B17" s="3"/>
+      <c r="C17" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E17" s="32" t="s">
+      <c r="E17" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="G17" s="32" t="s">
+      <c r="F17" s="3"/>
+      <c r="G17" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="I17" s="52" t="s">
+      <c r="I17" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="K17" s="32" t="s">
+      <c r="K17" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="L17" s="26"/>
-      <c r="M17" s="32" t="s">
+      <c r="L17" s="3"/>
+      <c r="M17" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="N17" s="26"/>
-      <c r="O17" s="32" t="s">
+      <c r="N17" s="3"/>
+      <c r="O17" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="P17" s="26"/>
-      <c r="Q17" s="33" t="s">
+      <c r="P17" s="3"/>
+      <c r="Q17" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="R17" s="30"/>
-      <c r="S17" s="32" t="s">
+      <c r="R17" s="7"/>
+      <c r="S17" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="T17" s="26"/>
-      <c r="U17" s="32" t="s">
+      <c r="T17" s="3"/>
+      <c r="U17" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="V17" s="26"/>
-      <c r="W17" s="32" t="s">
+      <c r="V17" s="3"/>
+      <c r="W17" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="X17" s="26"/>
+      <c r="X17" s="3"/>
       <c r="AA17"/>
       <c r="AB17"/>
       <c r="AC17"/>
@@ -2749,46 +2772,47 @@
       <c r="AI17"/>
     </row>
     <row r="18" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="32" t="s">
+      <c r="B18" s="3"/>
+      <c r="C18" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="G18" s="32" t="s">
+      <c r="F18" s="3"/>
+      <c r="G18" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="I18" s="52" t="s">
+      <c r="I18" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="K18" s="32" t="s">
+      <c r="K18" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="L18" s="26"/>
-      <c r="M18" s="34" t="s">
+      <c r="L18" s="3"/>
+      <c r="M18" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="N18" s="26"/>
-      <c r="O18" s="34" t="s">
+      <c r="N18" s="3"/>
+      <c r="O18" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="P18" s="26"/>
-      <c r="S18" s="32" t="s">
+      <c r="P18" s="3"/>
+      <c r="S18" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="T18" s="26"/>
-      <c r="U18" s="32" t="s">
+      <c r="T18" s="3"/>
+      <c r="U18" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="V18" s="26"/>
-      <c r="W18" s="33" t="s">
+      <c r="V18" s="3"/>
+      <c r="W18" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="X18" s="27"/>
+      <c r="X18" s="4"/>
       <c r="AA18"/>
       <c r="AB18"/>
       <c r="AC18"/>
@@ -2800,43 +2824,44 @@
       <c r="AI18"/>
     </row>
     <row r="19" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="26"/>
-      <c r="C19" s="33" t="s">
+      <c r="B19" s="3"/>
+      <c r="C19" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="30"/>
-      <c r="E19" s="32" t="s">
+      <c r="D19" s="7"/>
+      <c r="E19" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G19" s="32" t="s">
+      <c r="F19" s="3"/>
+      <c r="G19" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="I19" s="52" t="s">
+      <c r="I19" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="K19" s="32" t="s">
+      <c r="K19" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="L19" s="26"/>
-      <c r="M19" s="32" t="s">
+      <c r="L19" s="3"/>
+      <c r="M19" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="N19" s="26"/>
-      <c r="O19" s="32" t="s">
+      <c r="N19" s="3"/>
+      <c r="O19" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="P19" s="26"/>
-      <c r="S19" s="32" t="s">
+      <c r="P19" s="3"/>
+      <c r="S19" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="T19" s="26"/>
-      <c r="U19" s="32" t="s">
+      <c r="T19" s="3"/>
+      <c r="U19" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="V19" s="26"/>
+      <c r="V19" s="3"/>
       <c r="AA19"/>
       <c r="AB19"/>
       <c r="AC19"/>
@@ -2848,39 +2873,40 @@
       <c r="AI19"/>
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="E20" s="32" t="s">
+      <c r="B20" s="3"/>
+      <c r="E20" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G20" s="32" t="s">
+      <c r="F20" s="3"/>
+      <c r="G20" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="I20" s="52" t="s">
+      <c r="I20" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="K20" s="32" t="s">
+      <c r="K20" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="L20" s="26"/>
-      <c r="M20" s="34" t="s">
+      <c r="L20" s="3"/>
+      <c r="M20" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="N20" s="26"/>
-      <c r="O20" s="34" t="s">
+      <c r="N20" s="3"/>
+      <c r="O20" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="P20" s="26"/>
-      <c r="S20" s="32" t="s">
+      <c r="P20" s="3"/>
+      <c r="S20" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="T20" s="26"/>
-      <c r="U20" s="32" t="s">
+      <c r="T20" s="3"/>
+      <c r="U20" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="V20" s="26"/>
+      <c r="V20" s="3"/>
       <c r="AA20"/>
       <c r="AB20"/>
       <c r="AC20"/>
@@ -2892,39 +2918,40 @@
       <c r="AI20"/>
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A21" s="32" t="s">
+      <c r="A21" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="26"/>
-      <c r="E21" s="32" t="s">
+      <c r="B21" s="3"/>
+      <c r="E21" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="G21" s="32" t="s">
+      <c r="F21" s="3"/>
+      <c r="G21" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="I21" s="52" t="s">
+      <c r="I21" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="K21" s="32" t="s">
+      <c r="K21" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="L21" s="26"/>
-      <c r="M21" s="34" t="s">
+      <c r="L21" s="3"/>
+      <c r="M21" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="N21" s="26"/>
-      <c r="O21" s="34" t="s">
+      <c r="N21" s="3"/>
+      <c r="O21" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="P21" s="26"/>
-      <c r="S21" s="32" t="s">
+      <c r="P21" s="3"/>
+      <c r="S21" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="T21" s="26"/>
-      <c r="U21" s="32" t="s">
+      <c r="T21" s="3"/>
+      <c r="U21" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="V21" s="26"/>
+      <c r="V21" s="3"/>
       <c r="AA21"/>
       <c r="AB21"/>
       <c r="AC21"/>
@@ -2936,39 +2963,40 @@
       <c r="AI21"/>
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A22" s="32" t="s">
+      <c r="A22" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="26"/>
-      <c r="E22" s="32" t="s">
+      <c r="B22" s="3"/>
+      <c r="E22" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="G22" s="32" t="s">
+      <c r="F22" s="3"/>
+      <c r="G22" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="I22" s="52" t="s">
+      <c r="I22" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="K22" s="32" t="s">
+      <c r="K22" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="L22" s="26"/>
-      <c r="M22" s="34" t="s">
+      <c r="L22" s="3"/>
+      <c r="M22" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="N22" s="26"/>
-      <c r="O22" s="34" t="s">
+      <c r="N22" s="3"/>
+      <c r="O22" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="P22" s="26"/>
-      <c r="S22" s="32" t="s">
+      <c r="P22" s="3"/>
+      <c r="S22" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="T22" s="26"/>
-      <c r="U22" s="32" t="s">
+      <c r="T22" s="3"/>
+      <c r="U22" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="V22" s="26"/>
+      <c r="V22" s="3"/>
       <c r="AA22"/>
       <c r="AB22"/>
       <c r="AC22"/>
@@ -2979,41 +3007,43 @@
       <c r="AH22"/>
       <c r="AI22"/>
     </row>
-    <row r="23" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="32" t="s">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A23" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="26"/>
-      <c r="E23" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="F23" s="30"/>
-      <c r="G23" s="32" t="s">
+      <c r="B23" s="3"/>
+      <c r="E23" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="F23" s="3">
+        <v>1</v>
+      </c>
+      <c r="G23" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="I23" s="52" t="s">
+      <c r="I23" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="K23" s="32" t="s">
+      <c r="K23" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="L23" s="26"/>
-      <c r="M23" s="34" t="s">
+      <c r="L23" s="3"/>
+      <c r="M23" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="N23" s="26"/>
-      <c r="O23" s="34" t="s">
+      <c r="N23" s="3"/>
+      <c r="O23" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="P23" s="26"/>
-      <c r="S23" s="32" t="s">
+      <c r="P23" s="3"/>
+      <c r="S23" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="T23" s="26"/>
-      <c r="U23" s="32" t="s">
+      <c r="T23" s="3"/>
+      <c r="U23" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="V23" s="26"/>
+      <c r="V23" s="3"/>
       <c r="AA23"/>
       <c r="AB23"/>
       <c r="AC23"/>
@@ -3024,41 +3054,43 @@
       <c r="AH23"/>
       <c r="AI23"/>
     </row>
-    <row r="24" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="32" t="s">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="26"/>
-      <c r="E24" s="22" t="s">
-        <v>212</v>
-      </c>
-      <c r="F24" s="23"/>
-      <c r="G24" s="32" t="s">
+      <c r="B24" s="3"/>
+      <c r="E24" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="F24" s="3">
+        <v>1</v>
+      </c>
+      <c r="G24" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="I24" s="52" t="s">
+      <c r="I24" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="K24" s="32" t="s">
+      <c r="K24" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="L24" s="26"/>
-      <c r="M24" s="34" t="s">
+      <c r="L24" s="3"/>
+      <c r="M24" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="N24" s="26"/>
-      <c r="O24" s="34" t="s">
+      <c r="N24" s="3"/>
+      <c r="O24" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="P24" s="26"/>
-      <c r="S24" s="32" t="s">
+      <c r="P24" s="3"/>
+      <c r="S24" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="T24" s="26"/>
-      <c r="U24" s="32" t="s">
+      <c r="T24" s="3"/>
+      <c r="U24" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="V24" s="26"/>
+      <c r="V24" s="3"/>
       <c r="AA24"/>
       <c r="AB24"/>
       <c r="AC24"/>
@@ -3070,40 +3102,42 @@
       <c r="AI24"/>
     </row>
     <row r="25" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="26"/>
-      <c r="E25" s="63" t="s">
-        <v>198</v>
-      </c>
-      <c r="F25" s="25"/>
-      <c r="G25" s="34" t="s">
+      <c r="B25" s="3"/>
+      <c r="E25" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="F25" s="3">
+        <v>1</v>
+      </c>
+      <c r="G25" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="I25" s="52" t="s">
+      <c r="I25" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="K25" s="32" t="s">
+      <c r="K25" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="L25" s="26"/>
-      <c r="M25" s="34" t="s">
+      <c r="L25" s="3"/>
+      <c r="M25" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="N25" s="26"/>
-      <c r="O25" s="34" t="s">
+      <c r="N25" s="3"/>
+      <c r="O25" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="P25" s="26"/>
-      <c r="S25" s="32" t="s">
+      <c r="P25" s="3"/>
+      <c r="S25" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="T25" s="26"/>
-      <c r="U25" s="33" t="s">
+      <c r="T25" s="3"/>
+      <c r="U25" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="V25" s="27"/>
+      <c r="V25" s="4"/>
       <c r="AA25"/>
       <c r="AB25"/>
       <c r="AC25"/>
@@ -3115,36 +3149,38 @@
       <c r="AI25"/>
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="26"/>
-      <c r="E26" s="64" t="s">
-        <v>199</v>
-      </c>
-      <c r="F26" s="26"/>
-      <c r="G26" s="34" t="s">
+      <c r="B26" s="3"/>
+      <c r="E26" s="22" t="s">
+        <v>232</v>
+      </c>
+      <c r="F26" s="3">
+        <v>1.43279165</v>
+      </c>
+      <c r="G26" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="I26" s="52" t="s">
+      <c r="I26" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="K26" s="32" t="s">
+      <c r="K26" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="L26" s="26"/>
-      <c r="M26" s="34" t="s">
+      <c r="L26" s="3"/>
+      <c r="M26" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="N26" s="26"/>
-      <c r="O26" s="34" t="s">
+      <c r="N26" s="3"/>
+      <c r="O26" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="P26" s="26"/>
-      <c r="S26" s="32" t="s">
+      <c r="P26" s="3"/>
+      <c r="S26" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="T26" s="26"/>
+      <c r="T26" s="3"/>
       <c r="AA26"/>
       <c r="AB26"/>
       <c r="AC26"/>
@@ -3156,36 +3192,38 @@
       <c r="AI26"/>
     </row>
     <row r="27" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="32" t="s">
+      <c r="A27" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="26"/>
-      <c r="E27" s="64" t="s">
-        <v>200</v>
-      </c>
-      <c r="F27" s="26"/>
-      <c r="G27" s="34" t="s">
+      <c r="B27" s="3"/>
+      <c r="E27" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="F27" s="3">
+        <v>1</v>
+      </c>
+      <c r="G27" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="I27" s="52" t="s">
+      <c r="I27" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="K27" s="32" t="s">
+      <c r="K27" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="L27" s="26"/>
-      <c r="M27" s="34" t="s">
+      <c r="L27" s="3"/>
+      <c r="M27" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="N27" s="26"/>
-      <c r="O27" s="34" t="s">
+      <c r="N27" s="3"/>
+      <c r="O27" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="P27" s="26"/>
-      <c r="S27" s="33" t="s">
+      <c r="P27" s="3"/>
+      <c r="S27" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="T27" s="27"/>
+      <c r="T27" s="4"/>
       <c r="AA27"/>
       <c r="AB27"/>
       <c r="AC27"/>
@@ -3197,32 +3235,34 @@
       <c r="AI27"/>
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="26"/>
-      <c r="E28" s="64" t="s">
-        <v>201</v>
-      </c>
-      <c r="F28" s="26"/>
-      <c r="G28" s="34" t="s">
+      <c r="B28" s="3"/>
+      <c r="E28" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="F28" s="3">
+        <v>1</v>
+      </c>
+      <c r="G28" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I28" s="53" t="s">
+      <c r="I28" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="K28" s="32" t="s">
+      <c r="K28" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="L28" s="26"/>
-      <c r="M28" s="34" t="s">
+      <c r="L28" s="3"/>
+      <c r="M28" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="N28" s="26"/>
-      <c r="O28" s="34" t="s">
+      <c r="N28" s="3"/>
+      <c r="O28" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="P28" s="26"/>
+      <c r="P28" s="3"/>
       <c r="AA28"/>
       <c r="AB28"/>
       <c r="AC28"/>
@@ -3233,33 +3273,33 @@
       <c r="AH28"/>
       <c r="AI28"/>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A29" s="32" t="s">
+    <row r="29" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="E29" s="64" t="s">
-        <v>203</v>
-      </c>
-      <c r="F29" s="26"/>
-      <c r="G29" s="34" t="s">
+      <c r="B29" s="3"/>
+      <c r="E29" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F29" s="4"/>
+      <c r="G29" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="I29" s="53" t="s">
+      <c r="I29" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="K29" s="32" t="s">
+      <c r="K29" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="L29" s="26"/>
-      <c r="M29" s="34" t="s">
+      <c r="L29" s="3"/>
+      <c r="M29" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="N29" s="26"/>
-      <c r="O29" s="34" t="s">
+      <c r="N29" s="3"/>
+      <c r="O29" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="P29" s="26"/>
+      <c r="P29" s="3"/>
       <c r="AA29"/>
       <c r="AB29"/>
       <c r="AC29"/>
@@ -3270,33 +3310,33 @@
       <c r="AH29"/>
       <c r="AI29"/>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A30" s="32" t="s">
+    <row r="30" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="E30" s="64" t="s">
-        <v>202</v>
-      </c>
-      <c r="F30" s="26"/>
-      <c r="G30" s="34" t="s">
+      <c r="B30" s="3"/>
+      <c r="E30" s="34" t="s">
+        <v>212</v>
+      </c>
+      <c r="F30" s="36"/>
+      <c r="G30" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="I30" s="52" t="s">
+      <c r="I30" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="K30" s="32" t="s">
+      <c r="K30" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="L30" s="26"/>
-      <c r="M30" s="34" t="s">
+      <c r="L30" s="3"/>
+      <c r="M30" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="N30" s="26"/>
-      <c r="O30" s="34" t="s">
+      <c r="N30" s="3"/>
+      <c r="O30" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="P30" s="26"/>
+      <c r="P30" s="3"/>
       <c r="AA30"/>
       <c r="AB30"/>
       <c r="AC30"/>
@@ -3308,32 +3348,32 @@
       <c r="AI30"/>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A31" s="32" t="s">
+      <c r="A31" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="26"/>
-      <c r="E31" s="64" t="s">
-        <v>204</v>
-      </c>
-      <c r="F31" s="26"/>
-      <c r="G31" s="34" t="s">
+      <c r="B31" s="3"/>
+      <c r="E31" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="F31" s="2"/>
+      <c r="G31" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="I31" s="52" t="s">
+      <c r="I31" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="K31" s="32" t="s">
+      <c r="K31" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="L31" s="26"/>
-      <c r="M31" s="34" t="s">
+      <c r="L31" s="3"/>
+      <c r="M31" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="N31" s="26"/>
-      <c r="O31" s="34" t="s">
+      <c r="N31" s="3"/>
+      <c r="O31" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="P31" s="26"/>
+      <c r="P31" s="3"/>
       <c r="AA31"/>
       <c r="AB31"/>
       <c r="AC31"/>
@@ -3345,32 +3385,32 @@
       <c r="AI31"/>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A32" s="32" t="s">
+      <c r="A32" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="26"/>
-      <c r="E32" s="64" t="s">
-        <v>205</v>
-      </c>
-      <c r="F32" s="26"/>
-      <c r="G32" s="34" t="s">
+      <c r="B32" s="3"/>
+      <c r="E32" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="F32" s="3"/>
+      <c r="G32" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="I32" s="52" t="s">
+      <c r="I32" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="K32" s="32" t="s">
+      <c r="K32" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="L32" s="26"/>
-      <c r="M32" s="34" t="s">
+      <c r="L32" s="3"/>
+      <c r="M32" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="N32" s="26"/>
-      <c r="O32" s="34" t="s">
+      <c r="N32" s="3"/>
+      <c r="O32" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="P32" s="26"/>
+      <c r="P32" s="3"/>
       <c r="AA32"/>
       <c r="AB32"/>
       <c r="AC32"/>
@@ -3382,32 +3422,32 @@
       <c r="AI32"/>
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A33" s="32" t="s">
+      <c r="A33" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="26"/>
-      <c r="E33" s="64" t="s">
-        <v>206</v>
-      </c>
-      <c r="F33" s="26"/>
-      <c r="G33" s="34" t="s">
+      <c r="B33" s="3"/>
+      <c r="E33" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="F33" s="3"/>
+      <c r="G33" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="I33" s="53" t="s">
+      <c r="I33" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="K33" s="32" t="s">
+      <c r="K33" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="L33" s="26"/>
-      <c r="M33" s="34" t="s">
+      <c r="L33" s="3"/>
+      <c r="M33" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="N33" s="26"/>
-      <c r="O33" s="34" t="s">
+      <c r="N33" s="3"/>
+      <c r="O33" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="P33" s="26"/>
+      <c r="P33" s="3"/>
       <c r="AA33"/>
       <c r="AB33"/>
       <c r="AC33"/>
@@ -3419,33 +3459,33 @@
       <c r="AI33"/>
     </row>
     <row r="34" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="32" t="s">
+      <c r="A34" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="26"/>
-      <c r="E34" s="64" t="s">
-        <v>207</v>
-      </c>
-      <c r="F34" s="26"/>
-      <c r="G34" s="35" t="s">
+      <c r="B34" s="3"/>
+      <c r="E34" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="F34" s="3"/>
+      <c r="G34" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="H34" s="30"/>
-      <c r="I34" s="53" t="s">
+      <c r="H34" s="7"/>
+      <c r="I34" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="K34" s="32" t="s">
+      <c r="K34" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="L34" s="26"/>
-      <c r="M34" s="34" t="s">
+      <c r="L34" s="3"/>
+      <c r="M34" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="N34" s="26"/>
-      <c r="O34" s="34" t="s">
+      <c r="N34" s="3"/>
+      <c r="O34" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="P34" s="26"/>
+      <c r="P34" s="3"/>
       <c r="AA34"/>
       <c r="AB34"/>
       <c r="AC34"/>
@@ -3457,29 +3497,29 @@
       <c r="AI34"/>
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A35" s="32" t="s">
+      <c r="A35" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="26"/>
-      <c r="E35" s="64" t="s">
-        <v>208</v>
-      </c>
-      <c r="F35" s="26"/>
-      <c r="I35" s="53" t="s">
+      <c r="B35" s="3"/>
+      <c r="E35" s="22" t="s">
+        <v>203</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="I35" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="K35" s="32" t="s">
+      <c r="K35" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="L35" s="26"/>
-      <c r="M35" s="32" t="s">
+      <c r="L35" s="3"/>
+      <c r="M35" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="N35" s="26"/>
-      <c r="O35" s="32" t="s">
+      <c r="N35" s="3"/>
+      <c r="O35" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="P35" s="26"/>
+      <c r="P35" s="3"/>
       <c r="AA35"/>
       <c r="AB35"/>
       <c r="AC35"/>
@@ -3491,29 +3531,29 @@
       <c r="AI35"/>
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A36" s="32" t="s">
+      <c r="A36" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="26"/>
-      <c r="E36" s="64" t="s">
-        <v>209</v>
-      </c>
-      <c r="F36" s="26"/>
-      <c r="I36" s="53" t="s">
+      <c r="B36" s="3"/>
+      <c r="E36" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="F36" s="3"/>
+      <c r="I36" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="K36" s="32" t="s">
+      <c r="K36" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="L36" s="26"/>
-      <c r="M36" s="34" t="s">
+      <c r="L36" s="3"/>
+      <c r="M36" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="N36" s="26"/>
-      <c r="O36" s="34" t="s">
+      <c r="N36" s="3"/>
+      <c r="O36" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="P36" s="26"/>
+      <c r="P36" s="3"/>
       <c r="AA36"/>
       <c r="AB36"/>
       <c r="AC36"/>
@@ -3525,30 +3565,30 @@
       <c r="AI36"/>
     </row>
     <row r="37" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="32" t="s">
+      <c r="A37" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B37" s="26"/>
-      <c r="E37" s="64" t="s">
-        <v>210</v>
-      </c>
-      <c r="F37" s="26"/>
-      <c r="I37" s="54" t="s">
+      <c r="B37" s="3"/>
+      <c r="E37" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="F37" s="3"/>
+      <c r="I37" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="J37" s="30"/>
-      <c r="K37" s="32" t="s">
+      <c r="J37" s="7"/>
+      <c r="K37" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="L37" s="26"/>
-      <c r="M37" s="34" t="s">
+      <c r="L37" s="3"/>
+      <c r="M37" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="N37" s="26"/>
-      <c r="O37" s="34" t="s">
+      <c r="N37" s="3"/>
+      <c r="O37" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="P37" s="26"/>
+      <c r="P37" s="3"/>
       <c r="AA37"/>
       <c r="AB37"/>
       <c r="AC37"/>
@@ -3560,26 +3600,26 @@
       <c r="AI37"/>
     </row>
     <row r="38" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A38" s="32" t="s">
+      <c r="A38" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B38" s="26"/>
-      <c r="E38" s="64" t="s">
-        <v>211</v>
-      </c>
-      <c r="F38" s="26"/>
-      <c r="K38" s="32" t="s">
+      <c r="B38" s="3"/>
+      <c r="E38" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="F38" s="3"/>
+      <c r="K38" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="L38" s="26"/>
-      <c r="M38" s="34" t="s">
+      <c r="L38" s="3"/>
+      <c r="M38" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="N38" s="26"/>
-      <c r="O38" s="34" t="s">
+      <c r="N38" s="3"/>
+      <c r="O38" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="P38" s="26"/>
+      <c r="P38" s="3"/>
       <c r="AA38"/>
       <c r="AB38"/>
       <c r="AC38"/>
@@ -3591,22 +3631,22 @@
       <c r="AI38"/>
     </row>
     <row r="39" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="32" t="s">
+      <c r="A39" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B39" s="26"/>
-      <c r="E39" s="66" t="s">
-        <v>213</v>
-      </c>
-      <c r="F39" s="65"/>
-      <c r="K39" s="33" t="s">
+      <c r="B39" s="3"/>
+      <c r="E39" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="F39" s="3"/>
+      <c r="K39" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="L39" s="27"/>
-      <c r="M39" s="34"/>
-      <c r="N39" s="26"/>
-      <c r="O39" s="34"/>
-      <c r="P39" s="26"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="11"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="11"/>
+      <c r="P39" s="3"/>
       <c r="AA39"/>
       <c r="AB39"/>
       <c r="AC39"/>
@@ -3618,22 +3658,22 @@
       <c r="AI39"/>
     </row>
     <row r="40" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="32" t="s">
+      <c r="A40" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B40" s="26"/>
-      <c r="E40" s="66" t="s">
-        <v>214</v>
-      </c>
-      <c r="F40" s="26"/>
-      <c r="K40" s="22" t="s">
+      <c r="B40" s="3"/>
+      <c r="E40" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="F40" s="3"/>
+      <c r="K40" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="L40" s="55"/>
-      <c r="M40" s="55"/>
-      <c r="N40" s="55"/>
-      <c r="O40" s="55"/>
-      <c r="P40" s="23"/>
+      <c r="L40" s="35"/>
+      <c r="M40" s="35"/>
+      <c r="N40" s="35"/>
+      <c r="O40" s="35"/>
+      <c r="P40" s="36"/>
       <c r="AA40"/>
       <c r="AB40"/>
       <c r="AC40"/>
@@ -3645,22 +3685,22 @@
       <c r="AI40"/>
     </row>
     <row r="41" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A41" s="32" t="s">
+      <c r="A41" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B41" s="26"/>
-      <c r="E41" s="66" t="s">
-        <v>215</v>
-      </c>
-      <c r="F41" s="26"/>
-      <c r="K41" s="15" t="s">
+      <c r="B41" s="3"/>
+      <c r="E41" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="F41" s="3"/>
+      <c r="K41" s="37" t="s">
         <v>147</v>
       </c>
-      <c r="L41" s="10"/>
-      <c r="M41" s="48"/>
-      <c r="N41" s="49"/>
-      <c r="O41" s="10"/>
-      <c r="P41" s="16"/>
+      <c r="L41" s="38"/>
+      <c r="M41" s="39"/>
+      <c r="N41" s="43"/>
+      <c r="O41" s="38"/>
+      <c r="P41" s="40"/>
       <c r="AA41"/>
       <c r="AB41"/>
       <c r="AC41"/>
@@ -3672,22 +3712,22 @@
       <c r="AI41"/>
     </row>
     <row r="42" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A42" s="32" t="s">
+      <c r="A42" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B42" s="26"/>
-      <c r="E42" s="66" t="s">
-        <v>216</v>
-      </c>
-      <c r="F42" s="26"/>
-      <c r="K42" s="17" t="s">
+      <c r="B42" s="3"/>
+      <c r="E42" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="F42" s="3"/>
+      <c r="K42" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="L42" s="18"/>
-      <c r="M42" s="41"/>
-      <c r="N42" s="47"/>
-      <c r="O42" s="18"/>
-      <c r="P42" s="19"/>
+      <c r="L42" s="27"/>
+      <c r="M42" s="28"/>
+      <c r="N42" s="41"/>
+      <c r="O42" s="27"/>
+      <c r="P42" s="32"/>
       <c r="AA42"/>
       <c r="AB42"/>
       <c r="AC42"/>
@@ -3699,22 +3739,22 @@
       <c r="AI42"/>
     </row>
     <row r="43" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A43" s="32" t="s">
+      <c r="A43" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B43" s="26"/>
-      <c r="E43" s="66" t="s">
-        <v>217</v>
-      </c>
-      <c r="F43" s="26"/>
-      <c r="K43" s="17" t="s">
+      <c r="B43" s="3"/>
+      <c r="E43" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="F43" s="3"/>
+      <c r="K43" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="L43" s="18"/>
-      <c r="M43" s="41"/>
-      <c r="N43" s="47"/>
-      <c r="O43" s="18"/>
-      <c r="P43" s="19"/>
+      <c r="L43" s="27"/>
+      <c r="M43" s="28"/>
+      <c r="N43" s="41"/>
+      <c r="O43" s="27"/>
+      <c r="P43" s="32"/>
       <c r="AA43"/>
       <c r="AB43"/>
       <c r="AC43"/>
@@ -3725,23 +3765,23 @@
       <c r="AH43"/>
       <c r="AI43"/>
     </row>
-    <row r="44" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="32" t="s">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A44" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B44" s="26"/>
-      <c r="E44" s="67" t="s">
-        <v>218</v>
-      </c>
-      <c r="F44" s="27"/>
-      <c r="K44" s="37" t="s">
+      <c r="B44" s="3"/>
+      <c r="E44" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F44" s="3"/>
+      <c r="K44" s="44" t="s">
         <v>151</v>
       </c>
-      <c r="L44" s="38"/>
+      <c r="L44" s="45"/>
       <c r="M44" s="46"/>
-      <c r="N44" s="47"/>
-      <c r="O44" s="18"/>
-      <c r="P44" s="19"/>
+      <c r="N44" s="41"/>
+      <c r="O44" s="27"/>
+      <c r="P44" s="32"/>
       <c r="AA44"/>
       <c r="AB44"/>
       <c r="AC44"/>
@@ -3753,18 +3793,22 @@
       <c r="AI44"/>
     </row>
     <row r="45" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A45" s="32" t="s">
+      <c r="A45" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B45" s="26"/>
-      <c r="K45" s="17" t="s">
+      <c r="B45" s="3"/>
+      <c r="E45" s="24" t="s">
+        <v>213</v>
+      </c>
+      <c r="F45" s="23"/>
+      <c r="K45" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="L45" s="18"/>
-      <c r="M45" s="41"/>
-      <c r="N45" s="47"/>
-      <c r="O45" s="18"/>
-      <c r="P45" s="19"/>
+      <c r="L45" s="27"/>
+      <c r="M45" s="28"/>
+      <c r="N45" s="41"/>
+      <c r="O45" s="27"/>
+      <c r="P45" s="32"/>
       <c r="AA45"/>
       <c r="AB45"/>
       <c r="AC45"/>
@@ -3776,18 +3820,22 @@
       <c r="AI45"/>
     </row>
     <row r="46" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A46" s="32" t="s">
+      <c r="A46" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B46" s="26"/>
-      <c r="K46" s="17" t="s">
+      <c r="B46" s="3"/>
+      <c r="E46" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="F46" s="3"/>
+      <c r="K46" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="L46" s="18"/>
-      <c r="M46" s="41"/>
-      <c r="N46" s="47"/>
-      <c r="O46" s="18"/>
-      <c r="P46" s="19"/>
+      <c r="L46" s="27"/>
+      <c r="M46" s="28"/>
+      <c r="N46" s="41"/>
+      <c r="O46" s="27"/>
+      <c r="P46" s="32"/>
       <c r="AA46"/>
       <c r="AB46"/>
       <c r="AC46"/>
@@ -3799,18 +3847,22 @@
       <c r="AI46"/>
     </row>
     <row r="47" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A47" s="32" t="s">
+      <c r="A47" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B47" s="26"/>
-      <c r="K47" s="17" t="s">
+      <c r="B47" s="3"/>
+      <c r="E47" s="24" t="s">
+        <v>215</v>
+      </c>
+      <c r="F47" s="3"/>
+      <c r="K47" s="26" t="s">
         <v>154</v>
       </c>
-      <c r="L47" s="18"/>
-      <c r="M47" s="41"/>
-      <c r="N47" s="47"/>
-      <c r="O47" s="18"/>
-      <c r="P47" s="19"/>
+      <c r="L47" s="27"/>
+      <c r="M47" s="28"/>
+      <c r="N47" s="41"/>
+      <c r="O47" s="27"/>
+      <c r="P47" s="32"/>
       <c r="AA47"/>
       <c r="AB47"/>
       <c r="AC47"/>
@@ -3822,18 +3874,22 @@
       <c r="AI47"/>
     </row>
     <row r="48" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="33" t="s">
+      <c r="A48" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B48" s="27"/>
-      <c r="K48" s="17" t="s">
+      <c r="B48" s="4"/>
+      <c r="E48" s="24" t="s">
+        <v>216</v>
+      </c>
+      <c r="F48" s="3"/>
+      <c r="K48" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="L48" s="18"/>
-      <c r="M48" s="41"/>
-      <c r="N48" s="47"/>
-      <c r="O48" s="18"/>
-      <c r="P48" s="19"/>
+      <c r="L48" s="27"/>
+      <c r="M48" s="28"/>
+      <c r="N48" s="41"/>
+      <c r="O48" s="27"/>
+      <c r="P48" s="32"/>
       <c r="AA48"/>
       <c r="AB48"/>
       <c r="AC48"/>
@@ -3844,15 +3900,19 @@
       <c r="AH48"/>
       <c r="AI48"/>
     </row>
-    <row r="49" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K49" s="17" t="s">
+    <row r="49" spans="5:35" x14ac:dyDescent="0.3">
+      <c r="E49" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="F49" s="3"/>
+      <c r="K49" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="L49" s="18"/>
-      <c r="M49" s="41"/>
-      <c r="N49" s="47"/>
-      <c r="O49" s="18"/>
-      <c r="P49" s="19"/>
+      <c r="L49" s="27"/>
+      <c r="M49" s="28"/>
+      <c r="N49" s="41"/>
+      <c r="O49" s="27"/>
+      <c r="P49" s="32"/>
       <c r="AA49"/>
       <c r="AB49"/>
       <c r="AC49"/>
@@ -3863,15 +3923,19 @@
       <c r="AH49"/>
       <c r="AI49"/>
     </row>
-    <row r="50" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K50" s="17" t="s">
+    <row r="50" spans="5:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E50" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="F50" s="4"/>
+      <c r="K50" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="L50" s="18"/>
-      <c r="M50" s="41"/>
-      <c r="N50" s="47"/>
-      <c r="O50" s="18"/>
-      <c r="P50" s="19"/>
+      <c r="L50" s="27"/>
+      <c r="M50" s="28"/>
+      <c r="N50" s="41"/>
+      <c r="O50" s="27"/>
+      <c r="P50" s="32"/>
       <c r="AA50"/>
       <c r="AB50"/>
       <c r="AC50"/>
@@ -3882,15 +3946,15 @@
       <c r="AH50"/>
       <c r="AI50"/>
     </row>
-    <row r="51" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K51" s="17" t="s">
+    <row r="51" spans="5:35" x14ac:dyDescent="0.3">
+      <c r="K51" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="L51" s="18"/>
-      <c r="M51" s="41"/>
-      <c r="N51" s="47"/>
-      <c r="O51" s="18"/>
-      <c r="P51" s="19"/>
+      <c r="L51" s="27"/>
+      <c r="M51" s="28"/>
+      <c r="N51" s="41"/>
+      <c r="O51" s="27"/>
+      <c r="P51" s="32"/>
       <c r="AA51"/>
       <c r="AB51"/>
       <c r="AC51"/>
@@ -3901,15 +3965,15 @@
       <c r="AH51"/>
       <c r="AI51"/>
     </row>
-    <row r="52" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K52" s="17" t="s">
+    <row r="52" spans="5:35" x14ac:dyDescent="0.3">
+      <c r="K52" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="L52" s="18"/>
-      <c r="M52" s="41"/>
-      <c r="N52" s="47"/>
-      <c r="O52" s="18"/>
-      <c r="P52" s="19"/>
+      <c r="L52" s="27"/>
+      <c r="M52" s="28"/>
+      <c r="N52" s="41"/>
+      <c r="O52" s="27"/>
+      <c r="P52" s="32"/>
       <c r="AA52"/>
       <c r="AB52"/>
       <c r="AC52"/>
@@ -3920,15 +3984,15 @@
       <c r="AH52"/>
       <c r="AI52"/>
     </row>
-    <row r="53" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K53" s="17" t="s">
+    <row r="53" spans="5:35" x14ac:dyDescent="0.3">
+      <c r="K53" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="L53" s="18"/>
-      <c r="M53" s="41"/>
-      <c r="N53" s="47"/>
-      <c r="O53" s="18"/>
-      <c r="P53" s="19"/>
+      <c r="L53" s="27"/>
+      <c r="M53" s="28"/>
+      <c r="N53" s="41"/>
+      <c r="O53" s="27"/>
+      <c r="P53" s="32"/>
       <c r="AA53"/>
       <c r="AB53"/>
       <c r="AC53"/>
@@ -3939,15 +4003,15 @@
       <c r="AH53"/>
       <c r="AI53"/>
     </row>
-    <row r="54" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K54" s="17" t="s">
+    <row r="54" spans="5:35" x14ac:dyDescent="0.3">
+      <c r="K54" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="L54" s="18"/>
-      <c r="M54" s="41"/>
-      <c r="N54" s="47"/>
-      <c r="O54" s="18"/>
-      <c r="P54" s="19"/>
+      <c r="L54" s="27"/>
+      <c r="M54" s="28"/>
+      <c r="N54" s="41"/>
+      <c r="O54" s="27"/>
+      <c r="P54" s="32"/>
       <c r="AA54"/>
       <c r="AB54"/>
       <c r="AC54"/>
@@ -3958,15 +4022,15 @@
       <c r="AH54"/>
       <c r="AI54"/>
     </row>
-    <row r="55" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K55" s="17" t="s">
+    <row r="55" spans="5:35" x14ac:dyDescent="0.3">
+      <c r="K55" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="L55" s="18"/>
-      <c r="M55" s="41"/>
-      <c r="N55" s="47"/>
-      <c r="O55" s="18"/>
-      <c r="P55" s="19"/>
+      <c r="L55" s="27"/>
+      <c r="M55" s="28"/>
+      <c r="N55" s="41"/>
+      <c r="O55" s="27"/>
+      <c r="P55" s="32"/>
       <c r="AA55"/>
       <c r="AB55"/>
       <c r="AC55"/>
@@ -3977,15 +4041,15 @@
       <c r="AH55"/>
       <c r="AI55"/>
     </row>
-    <row r="56" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K56" s="17" t="s">
+    <row r="56" spans="5:35" x14ac:dyDescent="0.3">
+      <c r="K56" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="L56" s="18"/>
-      <c r="M56" s="41"/>
-      <c r="N56" s="47"/>
-      <c r="O56" s="18"/>
-      <c r="P56" s="19"/>
+      <c r="L56" s="27"/>
+      <c r="M56" s="28"/>
+      <c r="N56" s="41"/>
+      <c r="O56" s="27"/>
+      <c r="P56" s="32"/>
       <c r="AA56"/>
       <c r="AB56"/>
       <c r="AC56"/>
@@ -3996,15 +4060,15 @@
       <c r="AH56"/>
       <c r="AI56"/>
     </row>
-    <row r="57" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K57" s="17" t="s">
+    <row r="57" spans="5:35" x14ac:dyDescent="0.3">
+      <c r="K57" s="26" t="s">
         <v>164</v>
       </c>
-      <c r="L57" s="18"/>
-      <c r="M57" s="41"/>
-      <c r="N57" s="47"/>
-      <c r="O57" s="18"/>
-      <c r="P57" s="19"/>
+      <c r="L57" s="27"/>
+      <c r="M57" s="28"/>
+      <c r="N57" s="41"/>
+      <c r="O57" s="27"/>
+      <c r="P57" s="32"/>
       <c r="AA57"/>
       <c r="AB57"/>
       <c r="AC57"/>
@@ -4015,15 +4079,15 @@
       <c r="AH57"/>
       <c r="AI57"/>
     </row>
-    <row r="58" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K58" s="17" t="s">
+    <row r="58" spans="5:35" x14ac:dyDescent="0.3">
+      <c r="K58" s="26" t="s">
         <v>165</v>
       </c>
-      <c r="L58" s="18"/>
-      <c r="M58" s="41"/>
-      <c r="N58" s="47"/>
-      <c r="O58" s="18"/>
-      <c r="P58" s="19"/>
+      <c r="L58" s="27"/>
+      <c r="M58" s="28"/>
+      <c r="N58" s="41"/>
+      <c r="O58" s="27"/>
+      <c r="P58" s="32"/>
       <c r="AA58"/>
       <c r="AB58"/>
       <c r="AC58"/>
@@ -4034,15 +4098,15 @@
       <c r="AH58"/>
       <c r="AI58"/>
     </row>
-    <row r="59" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K59" s="17" t="s">
+    <row r="59" spans="5:35" x14ac:dyDescent="0.3">
+      <c r="K59" s="26" t="s">
         <v>166</v>
       </c>
-      <c r="L59" s="18"/>
-      <c r="M59" s="41"/>
-      <c r="N59" s="47"/>
-      <c r="O59" s="18"/>
-      <c r="P59" s="19"/>
+      <c r="L59" s="27"/>
+      <c r="M59" s="28"/>
+      <c r="N59" s="41"/>
+      <c r="O59" s="27"/>
+      <c r="P59" s="32"/>
       <c r="AA59"/>
       <c r="AB59"/>
       <c r="AC59"/>
@@ -4053,15 +4117,15 @@
       <c r="AH59"/>
       <c r="AI59"/>
     </row>
-    <row r="60" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K60" s="17" t="s">
+    <row r="60" spans="5:35" x14ac:dyDescent="0.3">
+      <c r="K60" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="L60" s="18"/>
-      <c r="M60" s="41"/>
-      <c r="N60" s="47"/>
-      <c r="O60" s="18"/>
-      <c r="P60" s="19"/>
+      <c r="L60" s="27"/>
+      <c r="M60" s="28"/>
+      <c r="N60" s="41"/>
+      <c r="O60" s="27"/>
+      <c r="P60" s="32"/>
       <c r="AA60"/>
       <c r="AB60"/>
       <c r="AC60"/>
@@ -4072,15 +4136,15 @@
       <c r="AH60"/>
       <c r="AI60"/>
     </row>
-    <row r="61" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K61" s="17" t="s">
+    <row r="61" spans="5:35" x14ac:dyDescent="0.3">
+      <c r="K61" s="26" t="s">
         <v>168</v>
       </c>
-      <c r="L61" s="18"/>
-      <c r="M61" s="41"/>
-      <c r="N61" s="47"/>
-      <c r="O61" s="18"/>
-      <c r="P61" s="19"/>
+      <c r="L61" s="27"/>
+      <c r="M61" s="28"/>
+      <c r="N61" s="41"/>
+      <c r="O61" s="27"/>
+      <c r="P61" s="32"/>
       <c r="AA61"/>
       <c r="AB61"/>
       <c r="AC61"/>
@@ -4091,15 +4155,15 @@
       <c r="AH61"/>
       <c r="AI61"/>
     </row>
-    <row r="62" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K62" s="17" t="s">
+    <row r="62" spans="5:35" x14ac:dyDescent="0.3">
+      <c r="K62" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="L62" s="18"/>
-      <c r="M62" s="41"/>
-      <c r="N62" s="47"/>
-      <c r="O62" s="18"/>
-      <c r="P62" s="19"/>
+      <c r="L62" s="27"/>
+      <c r="M62" s="28"/>
+      <c r="N62" s="41"/>
+      <c r="O62" s="27"/>
+      <c r="P62" s="32"/>
       <c r="AA62"/>
       <c r="AB62"/>
       <c r="AC62"/>
@@ -4110,15 +4174,15 @@
       <c r="AH62"/>
       <c r="AI62"/>
     </row>
-    <row r="63" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K63" s="17" t="s">
+    <row r="63" spans="5:35" x14ac:dyDescent="0.3">
+      <c r="K63" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="L63" s="18"/>
-      <c r="M63" s="41"/>
-      <c r="N63" s="47"/>
-      <c r="O63" s="18"/>
-      <c r="P63" s="19"/>
+      <c r="L63" s="27"/>
+      <c r="M63" s="28"/>
+      <c r="N63" s="41"/>
+      <c r="O63" s="27"/>
+      <c r="P63" s="32"/>
       <c r="AA63"/>
       <c r="AB63"/>
       <c r="AC63"/>
@@ -4129,15 +4193,15 @@
       <c r="AH63"/>
       <c r="AI63"/>
     </row>
-    <row r="64" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K64" s="17" t="s">
+    <row r="64" spans="5:35" x14ac:dyDescent="0.3">
+      <c r="K64" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="L64" s="18"/>
-      <c r="M64" s="41"/>
-      <c r="N64" s="47"/>
-      <c r="O64" s="18"/>
-      <c r="P64" s="19"/>
+      <c r="L64" s="27"/>
+      <c r="M64" s="28"/>
+      <c r="N64" s="41"/>
+      <c r="O64" s="27"/>
+      <c r="P64" s="32"/>
       <c r="AA64"/>
       <c r="AB64"/>
       <c r="AC64"/>
@@ -4149,14 +4213,14 @@
       <c r="AI64"/>
     </row>
     <row r="65" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K65" s="17" t="s">
+      <c r="K65" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="L65" s="18"/>
-      <c r="M65" s="41"/>
-      <c r="N65" s="47"/>
-      <c r="O65" s="18"/>
-      <c r="P65" s="19"/>
+      <c r="L65" s="27"/>
+      <c r="M65" s="28"/>
+      <c r="N65" s="41"/>
+      <c r="O65" s="27"/>
+      <c r="P65" s="32"/>
       <c r="AA65"/>
       <c r="AB65"/>
       <c r="AC65"/>
@@ -4168,14 +4232,14 @@
       <c r="AI65"/>
     </row>
     <row r="66" spans="11:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K66" s="20" t="s">
+      <c r="K66" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="L66" s="14"/>
-      <c r="M66" s="50"/>
-      <c r="N66" s="51"/>
-      <c r="O66" s="14"/>
-      <c r="P66" s="21"/>
+      <c r="L66" s="30"/>
+      <c r="M66" s="31"/>
+      <c r="N66" s="42"/>
+      <c r="O66" s="30"/>
+      <c r="P66" s="33"/>
       <c r="AA66"/>
       <c r="AB66"/>
       <c r="AC66"/>
@@ -4187,14 +4251,14 @@
       <c r="AI66"/>
     </row>
     <row r="67" spans="11:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K67" s="22" t="s">
+      <c r="K67" s="34" t="s">
         <v>219</v>
       </c>
-      <c r="L67" s="55"/>
-      <c r="M67" s="55"/>
-      <c r="N67" s="55"/>
-      <c r="O67" s="55"/>
-      <c r="P67" s="23"/>
+      <c r="L67" s="35"/>
+      <c r="M67" s="35"/>
+      <c r="N67" s="35"/>
+      <c r="O67" s="35"/>
+      <c r="P67" s="36"/>
       <c r="AA67"/>
       <c r="AB67"/>
       <c r="AC67"/>
@@ -4206,14 +4270,14 @@
       <c r="AI67"/>
     </row>
     <row r="68" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K68" s="15" t="s">
+      <c r="K68" s="37" t="s">
         <v>220</v>
       </c>
-      <c r="L68" s="10"/>
-      <c r="M68" s="48"/>
-      <c r="N68" s="10"/>
-      <c r="O68" s="10"/>
-      <c r="P68" s="16"/>
+      <c r="L68" s="38"/>
+      <c r="M68" s="39"/>
+      <c r="N68" s="38"/>
+      <c r="O68" s="38"/>
+      <c r="P68" s="40"/>
       <c r="AA68"/>
       <c r="AB68"/>
       <c r="AC68"/>
@@ -4225,14 +4289,14 @@
       <c r="AI68"/>
     </row>
     <row r="69" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K69" s="17" t="s">
+      <c r="K69" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="L69" s="18"/>
-      <c r="M69" s="41"/>
-      <c r="N69" s="18"/>
-      <c r="O69" s="18"/>
-      <c r="P69" s="19"/>
+      <c r="L69" s="27"/>
+      <c r="M69" s="28"/>
+      <c r="N69" s="27"/>
+      <c r="O69" s="27"/>
+      <c r="P69" s="32"/>
       <c r="AA69"/>
       <c r="AB69"/>
       <c r="AC69"/>
@@ -4244,14 +4308,14 @@
       <c r="AI69"/>
     </row>
     <row r="70" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K70" s="17" t="s">
+      <c r="K70" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="L70" s="18"/>
-      <c r="M70" s="41"/>
-      <c r="N70" s="18"/>
-      <c r="O70" s="18"/>
-      <c r="P70" s="19"/>
+      <c r="L70" s="27"/>
+      <c r="M70" s="28"/>
+      <c r="N70" s="27"/>
+      <c r="O70" s="27"/>
+      <c r="P70" s="32"/>
       <c r="AA70"/>
       <c r="AB70"/>
       <c r="AC70"/>
@@ -4263,14 +4327,14 @@
       <c r="AI70"/>
     </row>
     <row r="71" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K71" s="17" t="s">
+      <c r="K71" s="26" t="s">
         <v>223</v>
       </c>
-      <c r="L71" s="18"/>
-      <c r="M71" s="41"/>
-      <c r="N71" s="18"/>
-      <c r="O71" s="18"/>
-      <c r="P71" s="19"/>
+      <c r="L71" s="27"/>
+      <c r="M71" s="28"/>
+      <c r="N71" s="27"/>
+      <c r="O71" s="27"/>
+      <c r="P71" s="32"/>
       <c r="AA71"/>
       <c r="AB71"/>
       <c r="AC71"/>
@@ -4282,14 +4346,14 @@
       <c r="AI71"/>
     </row>
     <row r="72" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K72" s="17" t="s">
+      <c r="K72" s="26" t="s">
         <v>224</v>
       </c>
-      <c r="L72" s="18"/>
-      <c r="M72" s="41"/>
-      <c r="N72" s="18"/>
-      <c r="O72" s="18"/>
-      <c r="P72" s="19"/>
+      <c r="L72" s="27"/>
+      <c r="M72" s="28"/>
+      <c r="N72" s="27"/>
+      <c r="O72" s="27"/>
+      <c r="P72" s="32"/>
       <c r="AA72"/>
       <c r="AB72"/>
       <c r="AC72"/>
@@ -4301,14 +4365,14 @@
       <c r="AI72"/>
     </row>
     <row r="73" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K73" s="17" t="s">
+      <c r="K73" s="26" t="s">
         <v>225</v>
       </c>
-      <c r="L73" s="18"/>
-      <c r="M73" s="41"/>
-      <c r="N73" s="18"/>
-      <c r="O73" s="18"/>
-      <c r="P73" s="19"/>
+      <c r="L73" s="27"/>
+      <c r="M73" s="28"/>
+      <c r="N73" s="27"/>
+      <c r="O73" s="27"/>
+      <c r="P73" s="32"/>
       <c r="AA73"/>
       <c r="AB73"/>
       <c r="AC73"/>
@@ -4320,14 +4384,14 @@
       <c r="AI73"/>
     </row>
     <row r="74" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K74" s="17" t="s">
+      <c r="K74" s="26" t="s">
         <v>226</v>
       </c>
-      <c r="L74" s="18"/>
-      <c r="M74" s="41"/>
-      <c r="N74" s="18"/>
-      <c r="O74" s="18"/>
-      <c r="P74" s="19"/>
+      <c r="L74" s="27"/>
+      <c r="M74" s="28"/>
+      <c r="N74" s="27"/>
+      <c r="O74" s="27"/>
+      <c r="P74" s="32"/>
       <c r="AA74"/>
       <c r="AB74"/>
       <c r="AC74"/>
@@ -4339,14 +4403,14 @@
       <c r="AI74"/>
     </row>
     <row r="75" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K75" s="17" t="s">
+      <c r="K75" s="26" t="s">
         <v>227</v>
       </c>
-      <c r="L75" s="18"/>
-      <c r="M75" s="41"/>
-      <c r="N75" s="18"/>
-      <c r="O75" s="18"/>
-      <c r="P75" s="19"/>
+      <c r="L75" s="27"/>
+      <c r="M75" s="28"/>
+      <c r="N75" s="27"/>
+      <c r="O75" s="27"/>
+      <c r="P75" s="32"/>
       <c r="AA75"/>
       <c r="AB75"/>
       <c r="AC75"/>
@@ -4358,14 +4422,14 @@
       <c r="AI75"/>
     </row>
     <row r="76" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K76" s="17" t="s">
+      <c r="K76" s="26" t="s">
         <v>228</v>
       </c>
-      <c r="L76" s="18"/>
-      <c r="M76" s="41"/>
-      <c r="N76" s="18"/>
-      <c r="O76" s="18"/>
-      <c r="P76" s="19"/>
+      <c r="L76" s="27"/>
+      <c r="M76" s="28"/>
+      <c r="N76" s="27"/>
+      <c r="O76" s="27"/>
+      <c r="P76" s="32"/>
       <c r="AA76"/>
       <c r="AB76"/>
       <c r="AC76"/>
@@ -4377,14 +4441,14 @@
       <c r="AI76"/>
     </row>
     <row r="77" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K77" s="17" t="s">
+      <c r="K77" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="L77" s="18"/>
-      <c r="M77" s="41"/>
-      <c r="N77" s="18"/>
-      <c r="O77" s="18"/>
-      <c r="P77" s="19"/>
+      <c r="L77" s="27"/>
+      <c r="M77" s="28"/>
+      <c r="N77" s="27"/>
+      <c r="O77" s="27"/>
+      <c r="P77" s="32"/>
       <c r="AA77"/>
       <c r="AB77"/>
       <c r="AC77"/>
@@ -4396,14 +4460,14 @@
       <c r="AI77"/>
     </row>
     <row r="78" spans="11:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K78" s="20" t="s">
+      <c r="K78" s="29" t="s">
         <v>230</v>
       </c>
-      <c r="L78" s="14"/>
-      <c r="M78" s="50"/>
-      <c r="N78" s="14"/>
-      <c r="O78" s="14"/>
-      <c r="P78" s="21"/>
+      <c r="L78" s="30"/>
+      <c r="M78" s="31"/>
+      <c r="N78" s="30"/>
+      <c r="O78" s="30"/>
+      <c r="P78" s="33"/>
       <c r="AA78"/>
       <c r="AB78"/>
       <c r="AC78"/>
@@ -5175,46 +5239,49 @@
     </row>
   </sheetData>
   <mergeCells count="99">
-    <mergeCell ref="K77:M77"/>
-    <mergeCell ref="K78:M78"/>
-    <mergeCell ref="N77:P77"/>
-    <mergeCell ref="N78:P78"/>
-    <mergeCell ref="N74:P74"/>
-    <mergeCell ref="K75:M75"/>
-    <mergeCell ref="N75:P75"/>
-    <mergeCell ref="K76:M76"/>
-    <mergeCell ref="N76:P76"/>
-    <mergeCell ref="K71:M71"/>
-    <mergeCell ref="N71:P71"/>
-    <mergeCell ref="K72:M72"/>
-    <mergeCell ref="N72:P72"/>
-    <mergeCell ref="K73:M73"/>
-    <mergeCell ref="N73:P73"/>
-    <mergeCell ref="K67:P67"/>
-    <mergeCell ref="K68:M68"/>
-    <mergeCell ref="N68:P68"/>
-    <mergeCell ref="K74:M74"/>
-    <mergeCell ref="N69:P69"/>
-    <mergeCell ref="K70:M70"/>
-    <mergeCell ref="N70:P70"/>
-    <mergeCell ref="K69:M69"/>
-    <mergeCell ref="N61:P61"/>
-    <mergeCell ref="N62:P62"/>
-    <mergeCell ref="N63:P63"/>
-    <mergeCell ref="N64:P64"/>
-    <mergeCell ref="N65:P65"/>
-    <mergeCell ref="N66:P66"/>
-    <mergeCell ref="N55:P55"/>
-    <mergeCell ref="N56:P56"/>
-    <mergeCell ref="N57:P57"/>
-    <mergeCell ref="N58:P58"/>
-    <mergeCell ref="N59:P59"/>
-    <mergeCell ref="N60:P60"/>
-    <mergeCell ref="N49:P49"/>
-    <mergeCell ref="N50:P50"/>
-    <mergeCell ref="N51:P51"/>
-    <mergeCell ref="N52:P52"/>
-    <mergeCell ref="N53:P53"/>
+    <mergeCell ref="A1:Z3"/>
+    <mergeCell ref="A10:Z10"/>
+    <mergeCell ref="A4:Z4"/>
+    <mergeCell ref="A5:Z5"/>
+    <mergeCell ref="A6:Z6"/>
+    <mergeCell ref="A7:Z7"/>
+    <mergeCell ref="A8:Z8"/>
+    <mergeCell ref="A9:Z9"/>
+    <mergeCell ref="Y12:Z12"/>
+    <mergeCell ref="A11:Z11"/>
+    <mergeCell ref="K40:P40"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="U12:V12"/>
+    <mergeCell ref="W12:X12"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K52:M52"/>
+    <mergeCell ref="K41:M41"/>
+    <mergeCell ref="K42:M42"/>
+    <mergeCell ref="K43:M43"/>
+    <mergeCell ref="K44:M44"/>
+    <mergeCell ref="K45:M45"/>
+    <mergeCell ref="K46:M46"/>
+    <mergeCell ref="K47:M47"/>
+    <mergeCell ref="K48:M48"/>
+    <mergeCell ref="K49:M49"/>
+    <mergeCell ref="K50:M50"/>
+    <mergeCell ref="K51:M51"/>
+    <mergeCell ref="K64:M64"/>
+    <mergeCell ref="K53:M53"/>
+    <mergeCell ref="K54:M54"/>
+    <mergeCell ref="K55:M55"/>
+    <mergeCell ref="K56:M56"/>
+    <mergeCell ref="K57:M57"/>
+    <mergeCell ref="K58:M58"/>
     <mergeCell ref="N54:P54"/>
     <mergeCell ref="K65:M65"/>
     <mergeCell ref="K66:M66"/>
@@ -5231,49 +5298,46 @@
     <mergeCell ref="K61:M61"/>
     <mergeCell ref="K62:M62"/>
     <mergeCell ref="K63:M63"/>
-    <mergeCell ref="K64:M64"/>
-    <mergeCell ref="K53:M53"/>
-    <mergeCell ref="K54:M54"/>
-    <mergeCell ref="K55:M55"/>
-    <mergeCell ref="K56:M56"/>
-    <mergeCell ref="K57:M57"/>
-    <mergeCell ref="K58:M58"/>
-    <mergeCell ref="K47:M47"/>
-    <mergeCell ref="K48:M48"/>
-    <mergeCell ref="K49:M49"/>
-    <mergeCell ref="K50:M50"/>
-    <mergeCell ref="K51:M51"/>
-    <mergeCell ref="K52:M52"/>
-    <mergeCell ref="K41:M41"/>
-    <mergeCell ref="K42:M42"/>
-    <mergeCell ref="K43:M43"/>
-    <mergeCell ref="K44:M44"/>
-    <mergeCell ref="K45:M45"/>
-    <mergeCell ref="K46:M46"/>
-    <mergeCell ref="Y12:Z12"/>
-    <mergeCell ref="A11:Z11"/>
-    <mergeCell ref="K40:P40"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="S12:T12"/>
-    <mergeCell ref="U12:V12"/>
-    <mergeCell ref="W12:X12"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="A5:Z5"/>
-    <mergeCell ref="A6:Z6"/>
-    <mergeCell ref="A7:Z7"/>
-    <mergeCell ref="A8:Z8"/>
-    <mergeCell ref="A9:Z9"/>
-    <mergeCell ref="A1:Z3"/>
-    <mergeCell ref="A10:Z10"/>
-    <mergeCell ref="A4:Z4"/>
+    <mergeCell ref="N49:P49"/>
+    <mergeCell ref="N50:P50"/>
+    <mergeCell ref="N51:P51"/>
+    <mergeCell ref="N52:P52"/>
+    <mergeCell ref="N53:P53"/>
+    <mergeCell ref="N66:P66"/>
+    <mergeCell ref="N55:P55"/>
+    <mergeCell ref="N56:P56"/>
+    <mergeCell ref="N57:P57"/>
+    <mergeCell ref="N58:P58"/>
+    <mergeCell ref="N59:P59"/>
+    <mergeCell ref="N60:P60"/>
+    <mergeCell ref="N61:P61"/>
+    <mergeCell ref="N62:P62"/>
+    <mergeCell ref="N63:P63"/>
+    <mergeCell ref="N64:P64"/>
+    <mergeCell ref="N65:P65"/>
+    <mergeCell ref="K67:P67"/>
+    <mergeCell ref="K68:M68"/>
+    <mergeCell ref="N68:P68"/>
+    <mergeCell ref="K74:M74"/>
+    <mergeCell ref="N69:P69"/>
+    <mergeCell ref="K70:M70"/>
+    <mergeCell ref="N70:P70"/>
+    <mergeCell ref="K69:M69"/>
+    <mergeCell ref="K71:M71"/>
+    <mergeCell ref="N71:P71"/>
+    <mergeCell ref="K72:M72"/>
+    <mergeCell ref="N72:P72"/>
+    <mergeCell ref="K73:M73"/>
+    <mergeCell ref="N73:P73"/>
+    <mergeCell ref="K77:M77"/>
+    <mergeCell ref="K78:M78"/>
+    <mergeCell ref="N77:P77"/>
+    <mergeCell ref="N78:P78"/>
+    <mergeCell ref="N74:P74"/>
+    <mergeCell ref="K75:M75"/>
+    <mergeCell ref="N75:P75"/>
+    <mergeCell ref="K76:M76"/>
+    <mergeCell ref="N76:P76"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="42" fitToWidth="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
More work on HiLDE Calculator and TOP Calculator. Fixed a problem in HighLiftCalc inside LSAerodynamicManager. More tests on take-off and landing with repect to ATR-72 and B747-100B.
</commit_message>
<xml_diff>
--- a/DOCS/InputFile/JPAD_INPUT.xlsx
+++ b/DOCS/InputFile/JPAD_INPUT.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16828"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vittorio\Desktop\Materiale JPAD\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="384" yWindow="84" windowWidth="10500" windowHeight="2688"/>
   </bookViews>
@@ -21,7 +26,7 @@
     <author xml:space="preserve">Vittorio </author>
   </authors>
   <commentList>
-    <comment ref="G12" authorId="0">
+    <comment ref="G12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -45,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S25" authorId="0">
+    <comment ref="S25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -70,7 +75,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K33" authorId="0">
+    <comment ref="K33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -94,7 +99,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M33" authorId="0">
+    <comment ref="M33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -118,7 +123,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O33" authorId="0">
+    <comment ref="O33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -142,7 +147,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K35" authorId="0">
+    <comment ref="K35" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -166,7 +171,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M35" authorId="0">
+    <comment ref="M35" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -190,7 +195,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O35" authorId="0">
+    <comment ref="O35" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -214,7 +219,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K36" authorId="0">
+    <comment ref="K36" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -238,7 +243,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M36" authorId="0">
+    <comment ref="M36" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -262,7 +267,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O36" authorId="0">
+    <comment ref="O36" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -286,7 +291,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K37" authorId="0">
+    <comment ref="K37" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -310,7 +315,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K39" authorId="0">
+    <comment ref="K39" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -334,7 +339,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K70" authorId="0">
+    <comment ref="K70" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -358,7 +363,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K75" authorId="0">
+    <comment ref="K75" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -382,7 +387,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K76" authorId="0">
+    <comment ref="K76" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -411,7 +416,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="242">
   <si>
     <t>JPAD INPUT DATA</t>
   </si>
@@ -1122,13 +1127,28 @@
   </si>
   <si>
     <t>Kcontinous</t>
+  </si>
+  <si>
+    <t>COSTO ZERO</t>
+  </si>
+  <si>
+    <t>DEFINITO NEL CODICE</t>
+  </si>
+  <si>
+    <t>FATTO</t>
+  </si>
+  <si>
+    <t>DA FARE (LUNGO)</t>
+  </si>
+  <si>
+    <t>DA RIPROGETTARE (DIMENSIONAMENTO STATISTICO, CHECK VOLUME FUEL TANK)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1178,19 +1198,27 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1200,18 +1228,51 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -1496,166 +1557,239 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="19" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="24" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="25" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="26" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="16" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="15" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="26" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="13" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="14" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="15" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="26" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="16" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="17" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="16" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="17" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="40% - Colore 3" xfId="2" builtinId="39"/>
+    <cellStyle name="Colore 2" xfId="1" builtinId="33"/>
+    <cellStyle name="Colore 5" xfId="3" builtinId="45"/>
+    <cellStyle name="Colore 6" xfId="4" builtinId="49"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1663,6 +1797,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1711,7 +1848,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1744,9 +1881,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1779,6 +1933,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1960,70 +2131,70 @@
   </sheetPr>
   <dimension ref="A1:AI147"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:Z10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.77734375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.77734375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="17" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.44140625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="26.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.109375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="51.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.44140625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="46.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.109375" style="6" customWidth="1"/>
-    <col min="11" max="11" width="41.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.88671875" style="6"/>
-    <col min="13" max="13" width="37.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" style="6"/>
-    <col min="15" max="15" width="41.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.88671875" style="6"/>
-    <col min="17" max="17" width="17" style="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.21875" style="6" customWidth="1"/>
-    <col min="19" max="19" width="49.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.44140625" style="6" customWidth="1"/>
-    <col min="21" max="21" width="49.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.44140625" style="6" customWidth="1"/>
-    <col min="23" max="23" width="49.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.88671875" style="6" customWidth="1"/>
-    <col min="25" max="25" width="17" style="6" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.77734375" style="6" customWidth="1"/>
-    <col min="27" max="35" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="70.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.77734375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="17" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.44140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="26.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="51.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.44140625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="46.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.109375" style="5" customWidth="1"/>
+    <col min="11" max="11" width="41.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" style="5"/>
+    <col min="13" max="13" width="37.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.88671875" style="5"/>
+    <col min="15" max="15" width="41.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.88671875" style="5"/>
+    <col min="17" max="17" width="17" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.21875" style="5" customWidth="1"/>
+    <col min="19" max="19" width="49.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.44140625" style="5" customWidth="1"/>
+    <col min="21" max="21" width="49.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.44140625" style="5" customWidth="1"/>
+    <col min="23" max="23" width="49.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.88671875" style="5" customWidth="1"/>
+    <col min="25" max="25" width="17" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.77734375" style="5" customWidth="1"/>
+    <col min="27" max="35" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57"/>
-      <c r="P1" s="57"/>
-      <c r="Q1" s="57"/>
-      <c r="R1" s="57"/>
-      <c r="S1" s="57"/>
-      <c r="T1" s="57"/>
-      <c r="U1" s="57"/>
-      <c r="V1" s="57"/>
-      <c r="W1" s="57"/>
-      <c r="X1" s="57"/>
-      <c r="Y1" s="57"/>
-      <c r="Z1" s="58"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
+      <c r="O1" s="74"/>
+      <c r="P1" s="74"/>
+      <c r="Q1" s="74"/>
+      <c r="R1" s="74"/>
+      <c r="S1" s="74"/>
+      <c r="T1" s="74"/>
+      <c r="U1" s="74"/>
+      <c r="V1" s="74"/>
+      <c r="W1" s="74"/>
+      <c r="X1" s="74"/>
+      <c r="Y1" s="74"/>
+      <c r="Z1" s="75"/>
       <c r="AA1"/>
       <c r="AB1"/>
       <c r="AC1"/>
@@ -2035,32 +2206,32 @@
       <c r="AI1"/>
     </row>
     <row r="2" spans="1:35" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="59"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
-      <c r="O2" s="60"/>
-      <c r="P2" s="60"/>
-      <c r="Q2" s="60"/>
-      <c r="R2" s="60"/>
-      <c r="S2" s="60"/>
-      <c r="T2" s="60"/>
-      <c r="U2" s="60"/>
-      <c r="V2" s="60"/>
-      <c r="W2" s="60"/>
-      <c r="X2" s="60"/>
-      <c r="Y2" s="60"/>
-      <c r="Z2" s="61"/>
+      <c r="A2" s="76"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
+      <c r="N2" s="77"/>
+      <c r="O2" s="77"/>
+      <c r="P2" s="77"/>
+      <c r="Q2" s="77"/>
+      <c r="R2" s="77"/>
+      <c r="S2" s="77"/>
+      <c r="T2" s="77"/>
+      <c r="U2" s="77"/>
+      <c r="V2" s="77"/>
+      <c r="W2" s="77"/>
+      <c r="X2" s="77"/>
+      <c r="Y2" s="77"/>
+      <c r="Z2" s="78"/>
       <c r="AA2"/>
       <c r="AB2"/>
       <c r="AC2"/>
@@ -2072,32 +2243,32 @@
       <c r="AI2"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="62"/>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
-      <c r="L3" s="63"/>
-      <c r="M3" s="63"/>
-      <c r="N3" s="63"/>
-      <c r="O3" s="63"/>
-      <c r="P3" s="63"/>
-      <c r="Q3" s="63"/>
-      <c r="R3" s="63"/>
-      <c r="S3" s="63"/>
-      <c r="T3" s="63"/>
-      <c r="U3" s="63"/>
-      <c r="V3" s="63"/>
-      <c r="W3" s="63"/>
-      <c r="X3" s="63"/>
-      <c r="Y3" s="63"/>
-      <c r="Z3" s="64"/>
+      <c r="A3" s="79"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="80"/>
+      <c r="L3" s="80"/>
+      <c r="M3" s="80"/>
+      <c r="N3" s="80"/>
+      <c r="O3" s="80"/>
+      <c r="P3" s="80"/>
+      <c r="Q3" s="80"/>
+      <c r="R3" s="80"/>
+      <c r="S3" s="80"/>
+      <c r="T3" s="80"/>
+      <c r="U3" s="80"/>
+      <c r="V3" s="80"/>
+      <c r="W3" s="80"/>
+      <c r="X3" s="80"/>
+      <c r="Y3" s="80"/>
+      <c r="Z3" s="81"/>
       <c r="AA3"/>
       <c r="AB3"/>
       <c r="AC3"/>
@@ -2109,34 +2280,34 @@
       <c r="AI3"/>
     </row>
     <row r="4" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="66"/>
-      <c r="K4" s="66"/>
-      <c r="L4" s="66"/>
-      <c r="M4" s="66"/>
-      <c r="N4" s="66"/>
-      <c r="O4" s="66"/>
-      <c r="P4" s="66"/>
-      <c r="Q4" s="66"/>
-      <c r="R4" s="66"/>
-      <c r="S4" s="66"/>
-      <c r="T4" s="66"/>
-      <c r="U4" s="66"/>
-      <c r="V4" s="66"/>
-      <c r="W4" s="66"/>
-      <c r="X4" s="66"/>
-      <c r="Y4" s="66"/>
-      <c r="Z4" s="67"/>
+      <c r="B4" s="89"/>
+      <c r="C4" s="89"/>
+      <c r="D4" s="89"/>
+      <c r="E4" s="89"/>
+      <c r="F4" s="89"/>
+      <c r="G4" s="89"/>
+      <c r="H4" s="89"/>
+      <c r="I4" s="89"/>
+      <c r="J4" s="89"/>
+      <c r="K4" s="89"/>
+      <c r="L4" s="89"/>
+      <c r="M4" s="89"/>
+      <c r="N4" s="89"/>
+      <c r="O4" s="89"/>
+      <c r="P4" s="89"/>
+      <c r="Q4" s="89"/>
+      <c r="R4" s="89"/>
+      <c r="S4" s="89"/>
+      <c r="T4" s="89"/>
+      <c r="U4" s="89"/>
+      <c r="V4" s="89"/>
+      <c r="W4" s="89"/>
+      <c r="X4" s="89"/>
+      <c r="Y4" s="89"/>
+      <c r="Z4" s="90"/>
       <c r="AA4"/>
       <c r="AB4"/>
       <c r="AC4"/>
@@ -2148,34 +2319,34 @@
       <c r="AI4"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="51"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="51"/>
-      <c r="K5" s="51"/>
-      <c r="L5" s="51"/>
-      <c r="M5" s="51"/>
-      <c r="N5" s="51"/>
-      <c r="O5" s="51"/>
-      <c r="P5" s="51"/>
-      <c r="Q5" s="51"/>
-      <c r="R5" s="51"/>
-      <c r="S5" s="51"/>
-      <c r="T5" s="51"/>
-      <c r="U5" s="51"/>
-      <c r="V5" s="51"/>
-      <c r="W5" s="51"/>
-      <c r="X5" s="51"/>
-      <c r="Y5" s="51"/>
-      <c r="Z5" s="52"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
+      <c r="L5" s="83"/>
+      <c r="M5" s="83"/>
+      <c r="N5" s="83"/>
+      <c r="O5" s="83"/>
+      <c r="P5" s="83"/>
+      <c r="Q5" s="83"/>
+      <c r="R5" s="83"/>
+      <c r="S5" s="83"/>
+      <c r="T5" s="83"/>
+      <c r="U5" s="83"/>
+      <c r="V5" s="83"/>
+      <c r="W5" s="83"/>
+      <c r="X5" s="83"/>
+      <c r="Y5" s="83"/>
+      <c r="Z5" s="84"/>
       <c r="AA5"/>
       <c r="AB5"/>
       <c r="AC5"/>
@@ -2187,34 +2358,34 @@
       <c r="AI5"/>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="54"/>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="54"/>
-      <c r="M6" s="54"/>
-      <c r="N6" s="54"/>
-      <c r="O6" s="54"/>
-      <c r="P6" s="54"/>
-      <c r="Q6" s="54"/>
-      <c r="R6" s="54"/>
-      <c r="S6" s="54"/>
-      <c r="T6" s="54"/>
-      <c r="U6" s="54"/>
-      <c r="V6" s="54"/>
-      <c r="W6" s="54"/>
-      <c r="X6" s="54"/>
-      <c r="Y6" s="54"/>
-      <c r="Z6" s="55"/>
+      <c r="B6" s="86"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="86"/>
+      <c r="I6" s="86"/>
+      <c r="J6" s="86"/>
+      <c r="K6" s="86"/>
+      <c r="L6" s="86"/>
+      <c r="M6" s="86"/>
+      <c r="N6" s="86"/>
+      <c r="O6" s="86"/>
+      <c r="P6" s="86"/>
+      <c r="Q6" s="86"/>
+      <c r="R6" s="86"/>
+      <c r="S6" s="86"/>
+      <c r="T6" s="86"/>
+      <c r="U6" s="86"/>
+      <c r="V6" s="86"/>
+      <c r="W6" s="86"/>
+      <c r="X6" s="86"/>
+      <c r="Y6" s="86"/>
+      <c r="Z6" s="87"/>
       <c r="AA6"/>
       <c r="AB6"/>
       <c r="AC6"/>
@@ -2226,34 +2397,34 @@
       <c r="AI6"/>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="54"/>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="54"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="54"/>
-      <c r="J7" s="54"/>
-      <c r="K7" s="54"/>
-      <c r="L7" s="54"/>
-      <c r="M7" s="54"/>
-      <c r="N7" s="54"/>
-      <c r="O7" s="54"/>
-      <c r="P7" s="54"/>
-      <c r="Q7" s="54"/>
-      <c r="R7" s="54"/>
-      <c r="S7" s="54"/>
-      <c r="T7" s="54"/>
-      <c r="U7" s="54"/>
-      <c r="V7" s="54"/>
-      <c r="W7" s="54"/>
-      <c r="X7" s="54"/>
-      <c r="Y7" s="54"/>
-      <c r="Z7" s="55"/>
+      <c r="B7" s="86"/>
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="86"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="86"/>
+      <c r="L7" s="86"/>
+      <c r="M7" s="86"/>
+      <c r="N7" s="86"/>
+      <c r="O7" s="86"/>
+      <c r="P7" s="86"/>
+      <c r="Q7" s="86"/>
+      <c r="R7" s="86"/>
+      <c r="S7" s="86"/>
+      <c r="T7" s="86"/>
+      <c r="U7" s="86"/>
+      <c r="V7" s="86"/>
+      <c r="W7" s="86"/>
+      <c r="X7" s="86"/>
+      <c r="Y7" s="86"/>
+      <c r="Z7" s="87"/>
       <c r="AA7"/>
       <c r="AB7"/>
       <c r="AC7"/>
@@ -2265,34 +2436,34 @@
       <c r="AI7"/>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A8" s="53" t="s">
+      <c r="A8" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="54"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="54"/>
-      <c r="J8" s="54"/>
-      <c r="K8" s="54"/>
-      <c r="L8" s="54"/>
-      <c r="M8" s="54"/>
-      <c r="N8" s="54"/>
-      <c r="O8" s="54"/>
-      <c r="P8" s="54"/>
-      <c r="Q8" s="54"/>
-      <c r="R8" s="54"/>
-      <c r="S8" s="54"/>
-      <c r="T8" s="54"/>
-      <c r="U8" s="54"/>
-      <c r="V8" s="54"/>
-      <c r="W8" s="54"/>
-      <c r="X8" s="54"/>
-      <c r="Y8" s="54"/>
-      <c r="Z8" s="55"/>
+      <c r="B8" s="86"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="86"/>
+      <c r="H8" s="86"/>
+      <c r="I8" s="86"/>
+      <c r="J8" s="86"/>
+      <c r="K8" s="86"/>
+      <c r="L8" s="86"/>
+      <c r="M8" s="86"/>
+      <c r="N8" s="86"/>
+      <c r="O8" s="86"/>
+      <c r="P8" s="86"/>
+      <c r="Q8" s="86"/>
+      <c r="R8" s="86"/>
+      <c r="S8" s="86"/>
+      <c r="T8" s="86"/>
+      <c r="U8" s="86"/>
+      <c r="V8" s="86"/>
+      <c r="W8" s="86"/>
+      <c r="X8" s="86"/>
+      <c r="Y8" s="86"/>
+      <c r="Z8" s="87"/>
       <c r="AA8"/>
       <c r="AB8"/>
       <c r="AC8"/>
@@ -2304,34 +2475,34 @@
       <c r="AI8"/>
     </row>
     <row r="9" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="53" t="s">
+      <c r="A9" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="54"/>
-      <c r="C9" s="54"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="54"/>
-      <c r="I9" s="54"/>
-      <c r="J9" s="54"/>
-      <c r="K9" s="54"/>
-      <c r="L9" s="54"/>
-      <c r="M9" s="54"/>
-      <c r="N9" s="54"/>
-      <c r="O9" s="54"/>
-      <c r="P9" s="54"/>
-      <c r="Q9" s="54"/>
-      <c r="R9" s="54"/>
-      <c r="S9" s="54"/>
-      <c r="T9" s="54"/>
-      <c r="U9" s="54"/>
-      <c r="V9" s="54"/>
-      <c r="W9" s="54"/>
-      <c r="X9" s="54"/>
-      <c r="Y9" s="54"/>
-      <c r="Z9" s="55"/>
+      <c r="B9" s="86"/>
+      <c r="C9" s="86"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="86"/>
+      <c r="G9" s="86"/>
+      <c r="H9" s="86"/>
+      <c r="I9" s="86"/>
+      <c r="J9" s="86"/>
+      <c r="K9" s="86"/>
+      <c r="L9" s="86"/>
+      <c r="M9" s="86"/>
+      <c r="N9" s="86"/>
+      <c r="O9" s="86"/>
+      <c r="P9" s="86"/>
+      <c r="Q9" s="86"/>
+      <c r="R9" s="86"/>
+      <c r="S9" s="86"/>
+      <c r="T9" s="86"/>
+      <c r="U9" s="86"/>
+      <c r="V9" s="86"/>
+      <c r="W9" s="86"/>
+      <c r="X9" s="86"/>
+      <c r="Y9" s="86"/>
+      <c r="Z9" s="87"/>
       <c r="AA9"/>
       <c r="AB9"/>
       <c r="AC9"/>
@@ -2343,34 +2514,34 @@
       <c r="AI9"/>
     </row>
     <row r="10" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="65" t="s">
+      <c r="A10" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="66"/>
-      <c r="C10" s="66"/>
-      <c r="D10" s="66"/>
-      <c r="E10" s="66"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="66"/>
-      <c r="H10" s="66"/>
-      <c r="I10" s="66"/>
-      <c r="J10" s="66"/>
-      <c r="K10" s="66"/>
-      <c r="L10" s="66"/>
-      <c r="M10" s="66"/>
-      <c r="N10" s="66"/>
-      <c r="O10" s="66"/>
-      <c r="P10" s="66"/>
-      <c r="Q10" s="66"/>
-      <c r="R10" s="66"/>
-      <c r="S10" s="66"/>
-      <c r="T10" s="66"/>
-      <c r="U10" s="66"/>
-      <c r="V10" s="66"/>
-      <c r="W10" s="66"/>
-      <c r="X10" s="66"/>
-      <c r="Y10" s="66"/>
-      <c r="Z10" s="67"/>
+      <c r="B10" s="89"/>
+      <c r="C10" s="89"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="89"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="89"/>
+      <c r="H10" s="89"/>
+      <c r="I10" s="89"/>
+      <c r="J10" s="89"/>
+      <c r="K10" s="89"/>
+      <c r="L10" s="89"/>
+      <c r="M10" s="89"/>
+      <c r="N10" s="89"/>
+      <c r="O10" s="89"/>
+      <c r="P10" s="89"/>
+      <c r="Q10" s="89"/>
+      <c r="R10" s="89"/>
+      <c r="S10" s="89"/>
+      <c r="T10" s="89"/>
+      <c r="U10" s="89"/>
+      <c r="V10" s="89"/>
+      <c r="W10" s="89"/>
+      <c r="X10" s="89"/>
+      <c r="Y10" s="89"/>
+      <c r="Z10" s="90"/>
       <c r="AA10"/>
       <c r="AB10"/>
       <c r="AC10"/>
@@ -2381,89 +2552,89 @@
       <c r="AH10"/>
       <c r="AI10"/>
     </row>
-    <row r="11" spans="1:35" s="13" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="47" t="s">
+    <row r="11" spans="1:35" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="48"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
-      <c r="N11" s="48"/>
-      <c r="O11" s="48"/>
-      <c r="P11" s="48"/>
-      <c r="Q11" s="48"/>
-      <c r="R11" s="48"/>
-      <c r="S11" s="48"/>
-      <c r="T11" s="48"/>
-      <c r="U11" s="48"/>
-      <c r="V11" s="48"/>
-      <c r="W11" s="48"/>
-      <c r="X11" s="48"/>
-      <c r="Y11" s="48"/>
-      <c r="Z11" s="49"/>
+      <c r="B11" s="71"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="71"/>
+      <c r="H11" s="71"/>
+      <c r="I11" s="71"/>
+      <c r="J11" s="71"/>
+      <c r="K11" s="71"/>
+      <c r="L11" s="71"/>
+      <c r="M11" s="71"/>
+      <c r="N11" s="71"/>
+      <c r="O11" s="71"/>
+      <c r="P11" s="71"/>
+      <c r="Q11" s="71"/>
+      <c r="R11" s="71"/>
+      <c r="S11" s="71"/>
+      <c r="T11" s="71"/>
+      <c r="U11" s="71"/>
+      <c r="V11" s="71"/>
+      <c r="W11" s="71"/>
+      <c r="X11" s="71"/>
+      <c r="Y11" s="71"/>
+      <c r="Z11" s="72"/>
     </row>
     <row r="12" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="34" t="s">
+      <c r="B12" s="52"/>
+      <c r="C12" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="36"/>
-      <c r="E12" s="34" t="s">
+      <c r="D12" s="52"/>
+      <c r="E12" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="36"/>
-      <c r="G12" s="34" t="s">
+      <c r="F12" s="52"/>
+      <c r="G12" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="36"/>
-      <c r="I12" s="34" t="s">
+      <c r="H12" s="52"/>
+      <c r="I12" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="J12" s="36"/>
-      <c r="K12" s="34" t="s">
+      <c r="J12" s="52"/>
+      <c r="K12" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="L12" s="36"/>
-      <c r="M12" s="34" t="s">
+      <c r="L12" s="52"/>
+      <c r="M12" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="N12" s="36"/>
-      <c r="O12" s="34" t="s">
+      <c r="N12" s="52"/>
+      <c r="O12" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="P12" s="36"/>
-      <c r="Q12" s="34" t="s">
+      <c r="P12" s="52"/>
+      <c r="Q12" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="R12" s="36"/>
-      <c r="S12" s="34" t="s">
+      <c r="R12" s="52"/>
+      <c r="S12" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="T12" s="36"/>
-      <c r="U12" s="34" t="s">
+      <c r="T12" s="52"/>
+      <c r="U12" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="V12" s="36"/>
-      <c r="W12" s="34" t="s">
+      <c r="V12" s="52"/>
+      <c r="W12" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="X12" s="36"/>
-      <c r="Y12" s="34" t="s">
+      <c r="X12" s="52"/>
+      <c r="Y12" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="Z12" s="36"/>
+      <c r="Z12" s="52"/>
       <c r="AA12"/>
       <c r="AB12"/>
       <c r="AC12"/>
@@ -2475,58 +2646,58 @@
       <c r="AI12"/>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="8" t="s">
+      <c r="B13" s="1"/>
+      <c r="C13" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="8" t="s">
+      <c r="D13" s="4"/>
+      <c r="E13" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="68" t="s">
+      <c r="F13" s="1"/>
+      <c r="G13" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="H13" s="5"/>
-      <c r="I13" s="15" t="s">
+      <c r="H13" s="4"/>
+      <c r="I13" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="J13" s="5"/>
-      <c r="K13" s="1" t="s">
+      <c r="J13" s="4"/>
+      <c r="K13" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="L13" s="16"/>
-      <c r="M13" s="1" t="s">
+      <c r="L13" s="35"/>
+      <c r="M13" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="N13" s="16"/>
-      <c r="O13" s="1" t="s">
+      <c r="N13" s="35"/>
+      <c r="O13" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="8" t="s">
+      <c r="P13" s="35"/>
+      <c r="Q13" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="R13" s="5"/>
-      <c r="S13" s="8" t="s">
+      <c r="R13" s="4"/>
+      <c r="S13" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="T13" s="2"/>
-      <c r="U13" s="8" t="s">
+      <c r="T13" s="1"/>
+      <c r="U13" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="V13" s="2"/>
-      <c r="W13" s="8" t="s">
+      <c r="V13" s="1"/>
+      <c r="W13" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="X13" s="2"/>
-      <c r="Y13" s="8" t="s">
+      <c r="X13" s="1"/>
+      <c r="Y13" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="Z13" s="2"/>
+      <c r="Z13" s="1"/>
       <c r="AA13"/>
       <c r="AB13"/>
       <c r="AC13"/>
@@ -2538,55 +2709,55 @@
       <c r="AI13"/>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="9" t="s">
+      <c r="B14" s="2"/>
+      <c r="C14" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="11" t="s">
+      <c r="F14" s="2"/>
+      <c r="G14" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="H14" s="20"/>
-      <c r="I14" s="17" t="s">
+      <c r="H14" s="8"/>
+      <c r="I14" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="K14" s="9" t="s">
+      <c r="K14" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="L14" s="14"/>
-      <c r="M14" s="9" t="s">
+      <c r="L14" s="36"/>
+      <c r="M14" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="N14" s="3"/>
-      <c r="O14" s="9" t="s">
+      <c r="N14" s="37"/>
+      <c r="O14" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="9" t="s">
+      <c r="P14" s="37"/>
+      <c r="Q14" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="S14" s="9" t="s">
+      <c r="S14" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="T14" s="3"/>
-      <c r="U14" s="9" t="s">
+      <c r="T14" s="2"/>
+      <c r="U14" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="V14" s="3"/>
-      <c r="W14" s="9" t="s">
+      <c r="V14" s="2"/>
+      <c r="W14" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="X14" s="3"/>
-      <c r="Y14" s="9" t="s">
+      <c r="X14" s="2"/>
+      <c r="Y14" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="Z14" s="3"/>
+      <c r="Z14" s="2"/>
       <c r="AA14"/>
       <c r="AB14"/>
       <c r="AC14"/>
@@ -2598,54 +2769,54 @@
       <c r="AI14"/>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="9" t="s">
+      <c r="B15" s="2"/>
+      <c r="C15" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="11" t="s">
+      <c r="F15" s="2"/>
+      <c r="G15" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="I15" s="17" t="s">
+      <c r="I15" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="K15" s="9" t="s">
+      <c r="K15" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="L15" s="3"/>
-      <c r="M15" s="11" t="s">
+      <c r="L15" s="37"/>
+      <c r="M15" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="N15" s="3"/>
-      <c r="O15" s="11" t="s">
+      <c r="N15" s="37"/>
+      <c r="O15" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="9" t="s">
+      <c r="P15" s="37"/>
+      <c r="Q15" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="S15" s="9" t="s">
+      <c r="S15" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="T15" s="3"/>
-      <c r="U15" s="9" t="s">
+      <c r="T15" s="2"/>
+      <c r="U15" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="V15" s="3"/>
-      <c r="W15" s="9" t="s">
+      <c r="V15" s="2"/>
+      <c r="W15" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="X15" s="3"/>
-      <c r="Y15" s="9" t="s">
+      <c r="X15" s="2"/>
+      <c r="Y15" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="Z15" s="3"/>
+      <c r="Z15" s="2"/>
       <c r="AA15"/>
       <c r="AB15"/>
       <c r="AC15"/>
@@ -2657,54 +2828,54 @@
       <c r="AI15"/>
     </row>
     <row r="16" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="9" t="s">
+      <c r="B16" s="2"/>
+      <c r="C16" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="11" t="s">
+      <c r="F16" s="2"/>
+      <c r="G16" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="I16" s="17" t="s">
+      <c r="I16" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="K16" s="9" t="s">
+      <c r="K16" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="L16" s="3"/>
-      <c r="M16" s="11" t="s">
+      <c r="L16" s="37"/>
+      <c r="M16" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="N16" s="3"/>
-      <c r="O16" s="11" t="s">
+      <c r="N16" s="37"/>
+      <c r="O16" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="9" t="s">
+      <c r="P16" s="37"/>
+      <c r="Q16" s="33" t="s">
         <v>175</v>
       </c>
-      <c r="S16" s="9" t="s">
+      <c r="S16" s="33" t="s">
         <v>177</v>
       </c>
-      <c r="T16" s="3"/>
-      <c r="U16" s="9" t="s">
+      <c r="T16" s="2"/>
+      <c r="U16" s="33" t="s">
         <v>189</v>
       </c>
-      <c r="V16" s="3"/>
-      <c r="W16" s="9" t="s">
+      <c r="V16" s="2"/>
+      <c r="W16" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="X16" s="3"/>
-      <c r="Y16" s="10" t="s">
+      <c r="X16" s="2"/>
+      <c r="Y16" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="Z16" s="4"/>
+      <c r="Z16" s="3"/>
       <c r="AA16"/>
       <c r="AB16"/>
       <c r="AC16"/>
@@ -2716,51 +2887,51 @@
       <c r="AI16"/>
     </row>
     <row r="17" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="9" t="s">
+      <c r="B17" s="2"/>
+      <c r="C17" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="11" t="s">
+      <c r="F17" s="2"/>
+      <c r="G17" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="I17" s="17" t="s">
+      <c r="I17" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="K17" s="9" t="s">
+      <c r="K17" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="L17" s="3"/>
-      <c r="M17" s="9" t="s">
+      <c r="L17" s="37"/>
+      <c r="M17" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="N17" s="3"/>
-      <c r="O17" s="9" t="s">
+      <c r="N17" s="37"/>
+      <c r="O17" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="10" t="s">
+      <c r="P17" s="37"/>
+      <c r="Q17" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="R17" s="7"/>
-      <c r="S17" s="9" t="s">
+      <c r="R17" s="6"/>
+      <c r="S17" s="33" t="s">
         <v>178</v>
       </c>
-      <c r="T17" s="3"/>
-      <c r="U17" s="9" t="s">
+      <c r="T17" s="2"/>
+      <c r="U17" s="33" t="s">
         <v>190</v>
       </c>
-      <c r="V17" s="3"/>
-      <c r="W17" s="9" t="s">
+      <c r="V17" s="2"/>
+      <c r="W17" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="X17" s="3"/>
+      <c r="X17" s="2"/>
       <c r="AA17"/>
       <c r="AB17"/>
       <c r="AC17"/>
@@ -2772,47 +2943,47 @@
       <c r="AI17"/>
     </row>
     <row r="18" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="9" t="s">
+      <c r="B18" s="2"/>
+      <c r="C18" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="11" t="s">
+      <c r="F18" s="2"/>
+      <c r="G18" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="I18" s="17" t="s">
+      <c r="I18" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="K18" s="9" t="s">
+      <c r="K18" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="L18" s="3"/>
-      <c r="M18" s="11" t="s">
+      <c r="L18" s="37"/>
+      <c r="M18" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="N18" s="3"/>
-      <c r="O18" s="11" t="s">
+      <c r="N18" s="37"/>
+      <c r="O18" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="P18" s="3"/>
-      <c r="S18" s="9" t="s">
+      <c r="P18" s="37"/>
+      <c r="S18" s="33" t="s">
         <v>179</v>
       </c>
-      <c r="T18" s="3"/>
-      <c r="U18" s="9" t="s">
+      <c r="T18" s="2"/>
+      <c r="U18" s="33" t="s">
         <v>191</v>
       </c>
-      <c r="V18" s="3"/>
-      <c r="W18" s="10" t="s">
+      <c r="V18" s="2"/>
+      <c r="W18" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="X18" s="4"/>
+      <c r="X18" s="3"/>
       <c r="AA18"/>
       <c r="AB18"/>
       <c r="AC18"/>
@@ -2824,44 +2995,44 @@
       <c r="AI18"/>
     </row>
     <row r="19" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="10" t="s">
+      <c r="B19" s="2"/>
+      <c r="C19" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="9" t="s">
+      <c r="D19" s="6"/>
+      <c r="E19" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="11" t="s">
+      <c r="F19" s="2"/>
+      <c r="G19" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="I19" s="17" t="s">
+      <c r="I19" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="K19" s="9" t="s">
+      <c r="K19" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="L19" s="3"/>
-      <c r="M19" s="9" t="s">
+      <c r="L19" s="37"/>
+      <c r="M19" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="N19" s="3"/>
-      <c r="O19" s="9" t="s">
+      <c r="N19" s="37"/>
+      <c r="O19" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="P19" s="3"/>
-      <c r="S19" s="9" t="s">
+      <c r="P19" s="37"/>
+      <c r="S19" s="33" t="s">
         <v>180</v>
       </c>
-      <c r="T19" s="3"/>
-      <c r="U19" s="9" t="s">
+      <c r="T19" s="2"/>
+      <c r="U19" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="V19" s="3"/>
+      <c r="V19" s="2"/>
       <c r="AA19"/>
       <c r="AB19"/>
       <c r="AC19"/>
@@ -2873,40 +3044,40 @@
       <c r="AI19"/>
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="E20" s="9" t="s">
+      <c r="B20" s="2"/>
+      <c r="E20" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="11" t="s">
+      <c r="F20" s="2"/>
+      <c r="G20" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="I20" s="17" t="s">
+      <c r="I20" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="K20" s="9" t="s">
+      <c r="K20" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="L20" s="3"/>
-      <c r="M20" s="11" t="s">
+      <c r="L20" s="37"/>
+      <c r="M20" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="N20" s="3"/>
-      <c r="O20" s="11" t="s">
+      <c r="N20" s="37"/>
+      <c r="O20" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="P20" s="3"/>
-      <c r="S20" s="9" t="s">
+      <c r="P20" s="37"/>
+      <c r="S20" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="T20" s="3"/>
-      <c r="U20" s="9" t="s">
+      <c r="T20" s="2"/>
+      <c r="U20" s="33" t="s">
         <v>193</v>
       </c>
-      <c r="V20" s="3"/>
+      <c r="V20" s="2"/>
       <c r="AA20"/>
       <c r="AB20"/>
       <c r="AC20"/>
@@ -2918,40 +3089,40 @@
       <c r="AI20"/>
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="E21" s="9" t="s">
+      <c r="B21" s="2"/>
+      <c r="E21" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="11" t="s">
+      <c r="F21" s="2"/>
+      <c r="G21" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="I21" s="17" t="s">
+      <c r="I21" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="K21" s="9" t="s">
+      <c r="K21" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="L21" s="3"/>
-      <c r="M21" s="11" t="s">
+      <c r="L21" s="37"/>
+      <c r="M21" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="N21" s="3"/>
-      <c r="O21" s="11" t="s">
+      <c r="N21" s="37"/>
+      <c r="O21" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="P21" s="3"/>
-      <c r="S21" s="9" t="s">
+      <c r="P21" s="37"/>
+      <c r="S21" s="33" t="s">
         <v>182</v>
       </c>
-      <c r="T21" s="3"/>
-      <c r="U21" s="9" t="s">
+      <c r="T21" s="2"/>
+      <c r="U21" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="V21" s="3"/>
+      <c r="V21" s="2"/>
       <c r="AA21"/>
       <c r="AB21"/>
       <c r="AC21"/>
@@ -2963,40 +3134,40 @@
       <c r="AI21"/>
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="E22" s="9" t="s">
+      <c r="B22" s="2"/>
+      <c r="E22" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="3"/>
-      <c r="G22" s="11" t="s">
+      <c r="F22" s="2"/>
+      <c r="G22" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="I22" s="17" t="s">
+      <c r="I22" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="K22" s="9" t="s">
+      <c r="K22" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="L22" s="3"/>
-      <c r="M22" s="11" t="s">
+      <c r="L22" s="37"/>
+      <c r="M22" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="N22" s="3"/>
-      <c r="O22" s="11" t="s">
+      <c r="N22" s="37"/>
+      <c r="O22" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="P22" s="3"/>
-      <c r="S22" s="9" t="s">
+      <c r="P22" s="37"/>
+      <c r="S22" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="T22" s="3"/>
-      <c r="U22" s="9" t="s">
+      <c r="T22" s="2"/>
+      <c r="U22" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="V22" s="3"/>
+      <c r="V22" s="2"/>
       <c r="AA22"/>
       <c r="AB22"/>
       <c r="AC22"/>
@@ -3008,42 +3179,42 @@
       <c r="AI22"/>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="E23" s="9" t="s">
+      <c r="B23" s="2"/>
+      <c r="E23" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="2">
         <v>1</v>
       </c>
-      <c r="G23" s="11" t="s">
+      <c r="G23" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="I23" s="17" t="s">
+      <c r="I23" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="K23" s="9" t="s">
+      <c r="K23" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="L23" s="3"/>
-      <c r="M23" s="11" t="s">
+      <c r="L23" s="37"/>
+      <c r="M23" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="N23" s="3"/>
-      <c r="O23" s="11" t="s">
+      <c r="N23" s="37"/>
+      <c r="O23" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="P23" s="3"/>
-      <c r="S23" s="9" t="s">
+      <c r="P23" s="37"/>
+      <c r="S23" s="33" t="s">
         <v>184</v>
       </c>
-      <c r="T23" s="3"/>
-      <c r="U23" s="9" t="s">
+      <c r="T23" s="2"/>
+      <c r="U23" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="V23" s="3"/>
+      <c r="V23" s="2"/>
       <c r="AA23"/>
       <c r="AB23"/>
       <c r="AC23"/>
@@ -3055,42 +3226,42 @@
       <c r="AI23"/>
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="E24" s="9" t="s">
+      <c r="B24" s="2"/>
+      <c r="E24" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="2">
         <v>1</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="G24" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="I24" s="17" t="s">
+      <c r="I24" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="K24" s="9" t="s">
+      <c r="K24" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="L24" s="3"/>
-      <c r="M24" s="11" t="s">
+      <c r="L24" s="37"/>
+      <c r="M24" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="N24" s="3"/>
-      <c r="O24" s="11" t="s">
+      <c r="N24" s="37"/>
+      <c r="O24" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="P24" s="3"/>
-      <c r="S24" s="9" t="s">
+      <c r="P24" s="37"/>
+      <c r="S24" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="T24" s="3"/>
-      <c r="U24" s="9" t="s">
+      <c r="T24" s="2"/>
+      <c r="U24" s="33" t="s">
         <v>196</v>
       </c>
-      <c r="V24" s="3"/>
+      <c r="V24" s="2"/>
       <c r="AA24"/>
       <c r="AB24"/>
       <c r="AC24"/>
@@ -3102,42 +3273,42 @@
       <c r="AI24"/>
     </row>
     <row r="25" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="3"/>
-      <c r="E25" s="9" t="s">
+      <c r="B25" s="2"/>
+      <c r="E25" s="11" t="s">
         <v>236</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="2">
         <v>1</v>
       </c>
-      <c r="G25" s="11" t="s">
+      <c r="G25" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="I25" s="17" t="s">
+      <c r="I25" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="K25" s="9" t="s">
+      <c r="K25" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="L25" s="3"/>
-      <c r="M25" s="11" t="s">
+      <c r="L25" s="37"/>
+      <c r="M25" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="N25" s="3"/>
-      <c r="O25" s="11" t="s">
+      <c r="N25" s="37"/>
+      <c r="O25" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="P25" s="3"/>
-      <c r="S25" s="9" t="s">
+      <c r="P25" s="37"/>
+      <c r="S25" s="33" t="s">
         <v>186</v>
       </c>
-      <c r="T25" s="3"/>
-      <c r="U25" s="10" t="s">
+      <c r="T25" s="2"/>
+      <c r="U25" s="34" t="s">
         <v>188</v>
       </c>
-      <c r="V25" s="4"/>
+      <c r="V25" s="3"/>
       <c r="AA25"/>
       <c r="AB25"/>
       <c r="AC25"/>
@@ -3149,38 +3320,38 @@
       <c r="AI25"/>
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="E26" s="22" t="s">
+      <c r="B26" s="2"/>
+      <c r="E26" s="11" t="s">
         <v>232</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="2">
         <v>1.43279165</v>
       </c>
-      <c r="G26" s="11" t="s">
+      <c r="G26" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="I26" s="17" t="s">
+      <c r="I26" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="K26" s="9" t="s">
+      <c r="K26" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="L26" s="3"/>
-      <c r="M26" s="11" t="s">
+      <c r="L26" s="37"/>
+      <c r="M26" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="N26" s="3"/>
-      <c r="O26" s="11" t="s">
+      <c r="N26" s="37"/>
+      <c r="O26" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="P26" s="3"/>
-      <c r="S26" s="9" t="s">
+      <c r="P26" s="37"/>
+      <c r="S26" s="33" t="s">
         <v>187</v>
       </c>
-      <c r="T26" s="3"/>
+      <c r="T26" s="2"/>
       <c r="AA26"/>
       <c r="AB26"/>
       <c r="AC26"/>
@@ -3192,38 +3363,38 @@
       <c r="AI26"/>
     </row>
     <row r="27" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="3"/>
-      <c r="E27" s="9" t="s">
+      <c r="B27" s="2"/>
+      <c r="E27" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27" s="2">
         <v>1</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="G27" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="I27" s="17" t="s">
+      <c r="I27" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="K27" s="9" t="s">
+      <c r="K27" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="L27" s="3"/>
-      <c r="M27" s="11" t="s">
+      <c r="L27" s="37"/>
+      <c r="M27" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="N27" s="3"/>
-      <c r="O27" s="11" t="s">
+      <c r="N27" s="37"/>
+      <c r="O27" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="P27" s="3"/>
-      <c r="S27" s="10" t="s">
+      <c r="P27" s="37"/>
+      <c r="S27" s="34" t="s">
         <v>188</v>
       </c>
-      <c r="T27" s="4"/>
+      <c r="T27" s="3"/>
       <c r="AA27"/>
       <c r="AB27"/>
       <c r="AC27"/>
@@ -3235,34 +3406,34 @@
       <c r="AI27"/>
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="3"/>
-      <c r="E28" s="9" t="s">
+      <c r="B28" s="2"/>
+      <c r="E28" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28" s="2">
         <v>1</v>
       </c>
-      <c r="G28" s="11" t="s">
+      <c r="G28" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="I28" s="18" t="s">
+      <c r="I28" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="K28" s="9" t="s">
+      <c r="K28" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="L28" s="3"/>
-      <c r="M28" s="11" t="s">
+      <c r="L28" s="37"/>
+      <c r="M28" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="N28" s="3"/>
-      <c r="O28" s="11" t="s">
+      <c r="N28" s="37"/>
+      <c r="O28" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="P28" s="3"/>
+      <c r="P28" s="37"/>
       <c r="AA28"/>
       <c r="AB28"/>
       <c r="AC28"/>
@@ -3274,32 +3445,32 @@
       <c r="AI28"/>
     </row>
     <row r="29" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="E29" s="10" t="s">
+      <c r="B29" s="2"/>
+      <c r="E29" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="F29" s="4"/>
-      <c r="G29" s="11" t="s">
+      <c r="F29" s="3"/>
+      <c r="G29" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="I29" s="18" t="s">
+      <c r="I29" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="K29" s="9" t="s">
+      <c r="K29" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="L29" s="3"/>
-      <c r="M29" s="11" t="s">
+      <c r="L29" s="37"/>
+      <c r="M29" s="29" t="s">
         <v>135</v>
       </c>
-      <c r="N29" s="3"/>
-      <c r="O29" s="11" t="s">
+      <c r="N29" s="37"/>
+      <c r="O29" s="29" t="s">
         <v>135</v>
       </c>
-      <c r="P29" s="3"/>
+      <c r="P29" s="37"/>
       <c r="AA29"/>
       <c r="AB29"/>
       <c r="AC29"/>
@@ -3311,32 +3482,32 @@
       <c r="AI29"/>
     </row>
     <row r="30" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="3"/>
-      <c r="E30" s="34" t="s">
+      <c r="B30" s="2"/>
+      <c r="E30" s="50" t="s">
         <v>212</v>
       </c>
-      <c r="F30" s="36"/>
-      <c r="G30" s="11" t="s">
+      <c r="F30" s="52"/>
+      <c r="G30" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="I30" s="17" t="s">
+      <c r="I30" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="K30" s="9" t="s">
+      <c r="K30" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="L30" s="3"/>
-      <c r="M30" s="11" t="s">
+      <c r="L30" s="37"/>
+      <c r="M30" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="N30" s="3"/>
-      <c r="O30" s="11" t="s">
+      <c r="N30" s="37"/>
+      <c r="O30" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="P30" s="3"/>
+      <c r="P30" s="37"/>
       <c r="AA30"/>
       <c r="AB30"/>
       <c r="AC30"/>
@@ -3348,32 +3519,32 @@
       <c r="AI30"/>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="3"/>
-      <c r="E31" s="21" t="s">
+      <c r="B31" s="2"/>
+      <c r="E31" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="F31" s="2"/>
-      <c r="G31" s="11" t="s">
+      <c r="F31" s="1"/>
+      <c r="G31" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="I31" s="17" t="s">
+      <c r="I31" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="K31" s="9" t="s">
+      <c r="K31" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="L31" s="3"/>
-      <c r="M31" s="11" t="s">
+      <c r="L31" s="37"/>
+      <c r="M31" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="N31" s="3"/>
-      <c r="O31" s="11" t="s">
+      <c r="N31" s="37"/>
+      <c r="O31" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="P31" s="3"/>
+      <c r="P31" s="37"/>
       <c r="AA31"/>
       <c r="AB31"/>
       <c r="AC31"/>
@@ -3385,32 +3556,32 @@
       <c r="AI31"/>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="3"/>
-      <c r="E32" s="22" t="s">
+      <c r="B32" s="2"/>
+      <c r="E32" s="18" t="s">
         <v>199</v>
       </c>
-      <c r="F32" s="3"/>
-      <c r="G32" s="11" t="s">
+      <c r="F32" s="2"/>
+      <c r="G32" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="I32" s="17" t="s">
+      <c r="I32" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="K32" s="9" t="s">
+      <c r="K32" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="L32" s="3"/>
-      <c r="M32" s="11" t="s">
+      <c r="L32" s="37"/>
+      <c r="M32" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="N32" s="3"/>
-      <c r="O32" s="11" t="s">
+      <c r="N32" s="37"/>
+      <c r="O32" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="P32" s="3"/>
+      <c r="P32" s="37"/>
       <c r="AA32"/>
       <c r="AB32"/>
       <c r="AC32"/>
@@ -3422,32 +3593,32 @@
       <c r="AI32"/>
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="3"/>
-      <c r="E33" s="22" t="s">
+      <c r="B33" s="2"/>
+      <c r="E33" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="F33" s="3"/>
-      <c r="G33" s="11" t="s">
+      <c r="F33" s="2"/>
+      <c r="G33" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="I33" s="18" t="s">
+      <c r="I33" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="K33" s="9" t="s">
+      <c r="K33" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="L33" s="3"/>
-      <c r="M33" s="11" t="s">
+      <c r="L33" s="37"/>
+      <c r="M33" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="N33" s="3"/>
-      <c r="O33" s="11" t="s">
+      <c r="N33" s="37"/>
+      <c r="O33" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="P33" s="3"/>
+      <c r="P33" s="37"/>
       <c r="AA33"/>
       <c r="AB33"/>
       <c r="AC33"/>
@@ -3459,33 +3630,33 @@
       <c r="AI33"/>
     </row>
     <row r="34" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="3"/>
-      <c r="E34" s="22" t="s">
+      <c r="B34" s="2"/>
+      <c r="E34" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="F34" s="3"/>
-      <c r="G34" s="12" t="s">
+      <c r="F34" s="2"/>
+      <c r="G34" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="H34" s="7"/>
-      <c r="I34" s="18" t="s">
+      <c r="H34" s="6"/>
+      <c r="I34" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="K34" s="9" t="s">
+      <c r="K34" s="28" t="s">
         <v>140</v>
       </c>
-      <c r="L34" s="3"/>
-      <c r="M34" s="11" t="s">
+      <c r="L34" s="37"/>
+      <c r="M34" s="29" t="s">
         <v>140</v>
       </c>
-      <c r="N34" s="3"/>
-      <c r="O34" s="11" t="s">
+      <c r="N34" s="37"/>
+      <c r="O34" s="29" t="s">
         <v>140</v>
       </c>
-      <c r="P34" s="3"/>
+      <c r="P34" s="37"/>
       <c r="AA34"/>
       <c r="AB34"/>
       <c r="AC34"/>
@@ -3497,29 +3668,29 @@
       <c r="AI34"/>
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="3"/>
-      <c r="E35" s="22" t="s">
+      <c r="B35" s="2"/>
+      <c r="E35" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="F35" s="3"/>
-      <c r="I35" s="18" t="s">
+      <c r="F35" s="2"/>
+      <c r="I35" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="K35" s="9" t="s">
+      <c r="K35" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="L35" s="3"/>
-      <c r="M35" s="9" t="s">
+      <c r="L35" s="37"/>
+      <c r="M35" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="N35" s="3"/>
-      <c r="O35" s="9" t="s">
+      <c r="N35" s="37"/>
+      <c r="O35" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="P35" s="3"/>
+      <c r="P35" s="37"/>
       <c r="AA35"/>
       <c r="AB35"/>
       <c r="AC35"/>
@@ -3531,29 +3702,29 @@
       <c r="AI35"/>
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="3"/>
-      <c r="E36" s="22" t="s">
+      <c r="B36" s="2"/>
+      <c r="E36" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="F36" s="3"/>
-      <c r="I36" s="18" t="s">
+      <c r="F36" s="2"/>
+      <c r="I36" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="K36" s="9" t="s">
+      <c r="K36" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="L36" s="3"/>
-      <c r="M36" s="11" t="s">
+      <c r="L36" s="37"/>
+      <c r="M36" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="N36" s="3"/>
-      <c r="O36" s="11" t="s">
+      <c r="N36" s="37"/>
+      <c r="O36" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="P36" s="3"/>
+      <c r="P36" s="37"/>
       <c r="AA36"/>
       <c r="AB36"/>
       <c r="AC36"/>
@@ -3565,30 +3736,30 @@
       <c r="AI36"/>
     </row>
     <row r="37" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="9" t="s">
+      <c r="A37" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B37" s="3"/>
-      <c r="E37" s="22" t="s">
+      <c r="B37" s="2"/>
+      <c r="E37" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="F37" s="3"/>
-      <c r="I37" s="19" t="s">
+      <c r="F37" s="2"/>
+      <c r="I37" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="J37" s="7"/>
-      <c r="K37" s="9" t="s">
+      <c r="J37" s="6"/>
+      <c r="K37" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="L37" s="3"/>
-      <c r="M37" s="11" t="s">
+      <c r="L37" s="37"/>
+      <c r="M37" s="29" t="s">
         <v>174</v>
       </c>
-      <c r="N37" s="3"/>
-      <c r="O37" s="11" t="s">
+      <c r="N37" s="37"/>
+      <c r="O37" s="29" t="s">
         <v>174</v>
       </c>
-      <c r="P37" s="3"/>
+      <c r="P37" s="37"/>
       <c r="AA37"/>
       <c r="AB37"/>
       <c r="AC37"/>
@@ -3600,26 +3771,26 @@
       <c r="AI37"/>
     </row>
     <row r="38" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A38" s="9" t="s">
+      <c r="A38" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="B38" s="3"/>
-      <c r="E38" s="22" t="s">
+      <c r="B38" s="2"/>
+      <c r="E38" s="18" t="s">
         <v>205</v>
       </c>
-      <c r="F38" s="3"/>
-      <c r="K38" s="9" t="s">
+      <c r="F38" s="2"/>
+      <c r="K38" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="L38" s="3"/>
-      <c r="M38" s="11" t="s">
+      <c r="L38" s="37"/>
+      <c r="M38" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="N38" s="3"/>
-      <c r="O38" s="11" t="s">
+      <c r="N38" s="37"/>
+      <c r="O38" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="P38" s="3"/>
+      <c r="P38" s="37"/>
       <c r="AA38"/>
       <c r="AB38"/>
       <c r="AC38"/>
@@ -3631,22 +3802,22 @@
       <c r="AI38"/>
     </row>
     <row r="39" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="9" t="s">
+      <c r="A39" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B39" s="3"/>
-      <c r="E39" s="22" t="s">
+      <c r="B39" s="2"/>
+      <c r="E39" s="18" t="s">
         <v>206</v>
       </c>
-      <c r="F39" s="3"/>
-      <c r="K39" s="10" t="s">
+      <c r="F39" s="2"/>
+      <c r="K39" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="L39" s="4"/>
-      <c r="M39" s="11"/>
-      <c r="N39" s="3"/>
-      <c r="O39" s="11"/>
-      <c r="P39" s="3"/>
+      <c r="L39" s="38"/>
+      <c r="M39" s="29"/>
+      <c r="N39" s="37"/>
+      <c r="O39" s="29"/>
+      <c r="P39" s="37"/>
       <c r="AA39"/>
       <c r="AB39"/>
       <c r="AC39"/>
@@ -3658,22 +3829,22 @@
       <c r="AI39"/>
     </row>
     <row r="40" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B40" s="3"/>
-      <c r="E40" s="22" t="s">
+      <c r="B40" s="2"/>
+      <c r="E40" s="18" t="s">
         <v>207</v>
       </c>
-      <c r="F40" s="3"/>
-      <c r="K40" s="34" t="s">
+      <c r="F40" s="2"/>
+      <c r="K40" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="L40" s="35"/>
-      <c r="M40" s="35"/>
-      <c r="N40" s="35"/>
-      <c r="O40" s="35"/>
-      <c r="P40" s="36"/>
+      <c r="L40" s="51"/>
+      <c r="M40" s="51"/>
+      <c r="N40" s="51"/>
+      <c r="O40" s="51"/>
+      <c r="P40" s="52"/>
       <c r="AA40"/>
       <c r="AB40"/>
       <c r="AC40"/>
@@ -3685,22 +3856,22 @@
       <c r="AI40"/>
     </row>
     <row r="41" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A41" s="9" t="s">
+      <c r="A41" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B41" s="3"/>
-      <c r="E41" s="22" t="s">
+      <c r="B41" s="2"/>
+      <c r="E41" s="18" t="s">
         <v>208</v>
       </c>
-      <c r="F41" s="3"/>
-      <c r="K41" s="37" t="s">
+      <c r="F41" s="2"/>
+      <c r="K41" s="67" t="s">
         <v>147</v>
       </c>
-      <c r="L41" s="38"/>
-      <c r="M41" s="39"/>
-      <c r="N41" s="43"/>
-      <c r="O41" s="38"/>
-      <c r="P41" s="40"/>
+      <c r="L41" s="68"/>
+      <c r="M41" s="69"/>
+      <c r="N41" s="66"/>
+      <c r="O41" s="56"/>
+      <c r="P41" s="57"/>
       <c r="AA41"/>
       <c r="AB41"/>
       <c r="AC41"/>
@@ -3712,22 +3883,22 @@
       <c r="AI41"/>
     </row>
     <row r="42" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A42" s="9" t="s">
+      <c r="A42" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B42" s="3"/>
-      <c r="E42" s="22" t="s">
+      <c r="B42" s="2"/>
+      <c r="E42" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="F42" s="3"/>
-      <c r="K42" s="26" t="s">
+      <c r="F42" s="2"/>
+      <c r="K42" s="60" t="s">
         <v>149</v>
       </c>
-      <c r="L42" s="27"/>
-      <c r="M42" s="28"/>
-      <c r="N42" s="41"/>
-      <c r="O42" s="27"/>
-      <c r="P42" s="32"/>
+      <c r="L42" s="61"/>
+      <c r="M42" s="62"/>
+      <c r="N42" s="59"/>
+      <c r="O42" s="46"/>
+      <c r="P42" s="47"/>
       <c r="AA42"/>
       <c r="AB42"/>
       <c r="AC42"/>
@@ -3739,22 +3910,22 @@
       <c r="AI42"/>
     </row>
     <row r="43" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A43" s="9" t="s">
+      <c r="A43" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B43" s="3"/>
-      <c r="E43" s="22" t="s">
+      <c r="B43" s="2"/>
+      <c r="E43" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="F43" s="3"/>
-      <c r="K43" s="26" t="s">
+      <c r="F43" s="2"/>
+      <c r="K43" s="60" t="s">
         <v>150</v>
       </c>
-      <c r="L43" s="27"/>
-      <c r="M43" s="28"/>
-      <c r="N43" s="41"/>
-      <c r="O43" s="27"/>
-      <c r="P43" s="32"/>
+      <c r="L43" s="61"/>
+      <c r="M43" s="62"/>
+      <c r="N43" s="59"/>
+      <c r="O43" s="46"/>
+      <c r="P43" s="47"/>
       <c r="AA43"/>
       <c r="AB43"/>
       <c r="AC43"/>
@@ -3766,22 +3937,22 @@
       <c r="AI43"/>
     </row>
     <row r="44" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A44" s="9" t="s">
+      <c r="A44" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B44" s="3"/>
-      <c r="E44" s="22" t="s">
+      <c r="B44" s="2"/>
+      <c r="E44" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="F44" s="3"/>
-      <c r="K44" s="44" t="s">
+      <c r="F44" s="2"/>
+      <c r="K44" s="60" t="s">
         <v>151</v>
       </c>
-      <c r="L44" s="45"/>
-      <c r="M44" s="46"/>
-      <c r="N44" s="41"/>
-      <c r="O44" s="27"/>
-      <c r="P44" s="32"/>
+      <c r="L44" s="61"/>
+      <c r="M44" s="62"/>
+      <c r="N44" s="59"/>
+      <c r="O44" s="46"/>
+      <c r="P44" s="47"/>
       <c r="AA44"/>
       <c r="AB44"/>
       <c r="AC44"/>
@@ -3793,22 +3964,22 @@
       <c r="AI44"/>
     </row>
     <row r="45" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A45" s="9" t="s">
+      <c r="A45" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B45" s="3"/>
-      <c r="E45" s="24" t="s">
+      <c r="B45" s="2"/>
+      <c r="E45" s="19" t="s">
         <v>213</v>
       </c>
-      <c r="F45" s="23"/>
-      <c r="K45" s="26" t="s">
+      <c r="F45" s="9"/>
+      <c r="K45" s="60" t="s">
         <v>152</v>
       </c>
-      <c r="L45" s="27"/>
-      <c r="M45" s="28"/>
-      <c r="N45" s="41"/>
-      <c r="O45" s="27"/>
-      <c r="P45" s="32"/>
+      <c r="L45" s="61"/>
+      <c r="M45" s="62"/>
+      <c r="N45" s="59"/>
+      <c r="O45" s="46"/>
+      <c r="P45" s="47"/>
       <c r="AA45"/>
       <c r="AB45"/>
       <c r="AC45"/>
@@ -3820,22 +3991,22 @@
       <c r="AI45"/>
     </row>
     <row r="46" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A46" s="9" t="s">
+      <c r="A46" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B46" s="3"/>
-      <c r="E46" s="24" t="s">
+      <c r="B46" s="2"/>
+      <c r="E46" s="19" t="s">
         <v>214</v>
       </c>
-      <c r="F46" s="3"/>
-      <c r="K46" s="26" t="s">
+      <c r="F46" s="2"/>
+      <c r="K46" s="60" t="s">
         <v>153</v>
       </c>
-      <c r="L46" s="27"/>
-      <c r="M46" s="28"/>
-      <c r="N46" s="41"/>
-      <c r="O46" s="27"/>
-      <c r="P46" s="32"/>
+      <c r="L46" s="61"/>
+      <c r="M46" s="62"/>
+      <c r="N46" s="59"/>
+      <c r="O46" s="46"/>
+      <c r="P46" s="47"/>
       <c r="AA46"/>
       <c r="AB46"/>
       <c r="AC46"/>
@@ -3847,22 +4018,22 @@
       <c r="AI46"/>
     </row>
     <row r="47" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A47" s="9" t="s">
+      <c r="A47" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B47" s="3"/>
-      <c r="E47" s="24" t="s">
+      <c r="B47" s="2"/>
+      <c r="E47" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="F47" s="3"/>
-      <c r="K47" s="26" t="s">
+      <c r="F47" s="2"/>
+      <c r="K47" s="60" t="s">
         <v>154</v>
       </c>
-      <c r="L47" s="27"/>
-      <c r="M47" s="28"/>
-      <c r="N47" s="41"/>
-      <c r="O47" s="27"/>
-      <c r="P47" s="32"/>
+      <c r="L47" s="61"/>
+      <c r="M47" s="62"/>
+      <c r="N47" s="59"/>
+      <c r="O47" s="46"/>
+      <c r="P47" s="47"/>
       <c r="AA47"/>
       <c r="AB47"/>
       <c r="AC47"/>
@@ -3874,22 +4045,22 @@
       <c r="AI47"/>
     </row>
     <row r="48" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="10" t="s">
+      <c r="A48" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B48" s="4"/>
-      <c r="E48" s="24" t="s">
+      <c r="B48" s="3"/>
+      <c r="E48" s="21" t="s">
         <v>216</v>
       </c>
-      <c r="F48" s="3"/>
-      <c r="K48" s="26" t="s">
+      <c r="F48" s="2"/>
+      <c r="K48" s="60" t="s">
         <v>155</v>
       </c>
-      <c r="L48" s="27"/>
-      <c r="M48" s="28"/>
-      <c r="N48" s="41"/>
-      <c r="O48" s="27"/>
-      <c r="P48" s="32"/>
+      <c r="L48" s="61"/>
+      <c r="M48" s="62"/>
+      <c r="N48" s="59"/>
+      <c r="O48" s="46"/>
+      <c r="P48" s="47"/>
       <c r="AA48"/>
       <c r="AB48"/>
       <c r="AC48"/>
@@ -3900,19 +4071,19 @@
       <c r="AH48"/>
       <c r="AI48"/>
     </row>
-    <row r="49" spans="5:35" x14ac:dyDescent="0.3">
-      <c r="E49" s="24" t="s">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="E49" s="19" t="s">
         <v>217</v>
       </c>
-      <c r="F49" s="3"/>
-      <c r="K49" s="26" t="s">
+      <c r="F49" s="2"/>
+      <c r="K49" s="60" t="s">
         <v>156</v>
       </c>
-      <c r="L49" s="27"/>
-      <c r="M49" s="28"/>
-      <c r="N49" s="41"/>
-      <c r="O49" s="27"/>
-      <c r="P49" s="32"/>
+      <c r="L49" s="61"/>
+      <c r="M49" s="62"/>
+      <c r="N49" s="59"/>
+      <c r="O49" s="46"/>
+      <c r="P49" s="47"/>
       <c r="AA49"/>
       <c r="AB49"/>
       <c r="AC49"/>
@@ -3923,19 +4094,19 @@
       <c r="AH49"/>
       <c r="AI49"/>
     </row>
-    <row r="50" spans="5:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E50" s="25" t="s">
+    <row r="50" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E50" s="22" t="s">
         <v>218</v>
       </c>
-      <c r="F50" s="4"/>
-      <c r="K50" s="26" t="s">
+      <c r="F50" s="3"/>
+      <c r="K50" s="60" t="s">
         <v>157</v>
       </c>
-      <c r="L50" s="27"/>
-      <c r="M50" s="28"/>
-      <c r="N50" s="41"/>
-      <c r="O50" s="27"/>
-      <c r="P50" s="32"/>
+      <c r="L50" s="61"/>
+      <c r="M50" s="62"/>
+      <c r="N50" s="59"/>
+      <c r="O50" s="46"/>
+      <c r="P50" s="47"/>
       <c r="AA50"/>
       <c r="AB50"/>
       <c r="AC50"/>
@@ -3946,15 +4117,15 @@
       <c r="AH50"/>
       <c r="AI50"/>
     </row>
-    <row r="51" spans="5:35" x14ac:dyDescent="0.3">
-      <c r="K51" s="26" t="s">
+    <row r="51" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="K51" s="60" t="s">
         <v>158</v>
       </c>
-      <c r="L51" s="27"/>
-      <c r="M51" s="28"/>
-      <c r="N51" s="41"/>
-      <c r="O51" s="27"/>
-      <c r="P51" s="32"/>
+      <c r="L51" s="61"/>
+      <c r="M51" s="62"/>
+      <c r="N51" s="59"/>
+      <c r="O51" s="46"/>
+      <c r="P51" s="47"/>
       <c r="AA51"/>
       <c r="AB51"/>
       <c r="AC51"/>
@@ -3965,15 +4136,15 @@
       <c r="AH51"/>
       <c r="AI51"/>
     </row>
-    <row r="52" spans="5:35" x14ac:dyDescent="0.3">
-      <c r="K52" s="26" t="s">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="K52" s="60" t="s">
         <v>159</v>
       </c>
-      <c r="L52" s="27"/>
-      <c r="M52" s="28"/>
-      <c r="N52" s="41"/>
-      <c r="O52" s="27"/>
-      <c r="P52" s="32"/>
+      <c r="L52" s="61"/>
+      <c r="M52" s="62"/>
+      <c r="N52" s="59"/>
+      <c r="O52" s="46"/>
+      <c r="P52" s="47"/>
       <c r="AA52"/>
       <c r="AB52"/>
       <c r="AC52"/>
@@ -3984,15 +4155,15 @@
       <c r="AH52"/>
       <c r="AI52"/>
     </row>
-    <row r="53" spans="5:35" x14ac:dyDescent="0.3">
-      <c r="K53" s="26" t="s">
+    <row r="53" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="K53" s="60" t="s">
         <v>160</v>
       </c>
-      <c r="L53" s="27"/>
-      <c r="M53" s="28"/>
-      <c r="N53" s="41"/>
-      <c r="O53" s="27"/>
-      <c r="P53" s="32"/>
+      <c r="L53" s="61"/>
+      <c r="M53" s="62"/>
+      <c r="N53" s="59"/>
+      <c r="O53" s="46"/>
+      <c r="P53" s="47"/>
       <c r="AA53"/>
       <c r="AB53"/>
       <c r="AC53"/>
@@ -4003,15 +4174,15 @@
       <c r="AH53"/>
       <c r="AI53"/>
     </row>
-    <row r="54" spans="5:35" x14ac:dyDescent="0.3">
-      <c r="K54" s="26" t="s">
+    <row r="54" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K54" s="60" t="s">
         <v>161</v>
       </c>
-      <c r="L54" s="27"/>
-      <c r="M54" s="28"/>
-      <c r="N54" s="41"/>
-      <c r="O54" s="27"/>
-      <c r="P54" s="32"/>
+      <c r="L54" s="61"/>
+      <c r="M54" s="62"/>
+      <c r="N54" s="59"/>
+      <c r="O54" s="46"/>
+      <c r="P54" s="47"/>
       <c r="AA54"/>
       <c r="AB54"/>
       <c r="AC54"/>
@@ -4022,15 +4193,18 @@
       <c r="AH54"/>
       <c r="AI54"/>
     </row>
-    <row r="55" spans="5:35" x14ac:dyDescent="0.3">
-      <c r="K55" s="26" t="s">
+    <row r="55" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="K55" s="60" t="s">
         <v>162</v>
       </c>
-      <c r="L55" s="27"/>
-      <c r="M55" s="28"/>
-      <c r="N55" s="41"/>
-      <c r="O55" s="27"/>
-      <c r="P55" s="32"/>
+      <c r="L55" s="61"/>
+      <c r="M55" s="62"/>
+      <c r="N55" s="59"/>
+      <c r="O55" s="46"/>
+      <c r="P55" s="47"/>
       <c r="AA55"/>
       <c r="AB55"/>
       <c r="AC55"/>
@@ -4041,15 +4215,18 @@
       <c r="AH55"/>
       <c r="AI55"/>
     </row>
-    <row r="56" spans="5:35" x14ac:dyDescent="0.3">
-      <c r="K56" s="26" t="s">
+    <row r="56" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="K56" s="60" t="s">
         <v>163</v>
       </c>
-      <c r="L56" s="27"/>
-      <c r="M56" s="28"/>
-      <c r="N56" s="41"/>
-      <c r="O56" s="27"/>
-      <c r="P56" s="32"/>
+      <c r="L56" s="61"/>
+      <c r="M56" s="62"/>
+      <c r="N56" s="59"/>
+      <c r="O56" s="46"/>
+      <c r="P56" s="47"/>
       <c r="AA56"/>
       <c r="AB56"/>
       <c r="AC56"/>
@@ -4060,15 +4237,18 @@
       <c r="AH56"/>
       <c r="AI56"/>
     </row>
-    <row r="57" spans="5:35" x14ac:dyDescent="0.3">
-      <c r="K57" s="26" t="s">
+    <row r="57" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="26" t="s">
+        <v>239</v>
+      </c>
+      <c r="K57" s="60" t="s">
         <v>164</v>
       </c>
-      <c r="L57" s="27"/>
-      <c r="M57" s="28"/>
-      <c r="N57" s="41"/>
-      <c r="O57" s="27"/>
-      <c r="P57" s="32"/>
+      <c r="L57" s="61"/>
+      <c r="M57" s="62"/>
+      <c r="N57" s="59"/>
+      <c r="O57" s="46"/>
+      <c r="P57" s="47"/>
       <c r="AA57"/>
       <c r="AB57"/>
       <c r="AC57"/>
@@ -4079,15 +4259,18 @@
       <c r="AH57"/>
       <c r="AI57"/>
     </row>
-    <row r="58" spans="5:35" x14ac:dyDescent="0.3">
-      <c r="K58" s="26" t="s">
+    <row r="58" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="31" t="s">
+        <v>240</v>
+      </c>
+      <c r="K58" s="60" t="s">
         <v>165</v>
       </c>
-      <c r="L58" s="27"/>
-      <c r="M58" s="28"/>
-      <c r="N58" s="41"/>
-      <c r="O58" s="27"/>
-      <c r="P58" s="32"/>
+      <c r="L58" s="61"/>
+      <c r="M58" s="62"/>
+      <c r="N58" s="59"/>
+      <c r="O58" s="46"/>
+      <c r="P58" s="47"/>
       <c r="AA58"/>
       <c r="AB58"/>
       <c r="AC58"/>
@@ -4098,15 +4281,18 @@
       <c r="AH58"/>
       <c r="AI58"/>
     </row>
-    <row r="59" spans="5:35" x14ac:dyDescent="0.3">
-      <c r="K59" s="26" t="s">
+    <row r="59" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="39" t="s">
+        <v>241</v>
+      </c>
+      <c r="K59" s="60" t="s">
         <v>166</v>
       </c>
-      <c r="L59" s="27"/>
-      <c r="M59" s="28"/>
-      <c r="N59" s="41"/>
-      <c r="O59" s="27"/>
-      <c r="P59" s="32"/>
+      <c r="L59" s="61"/>
+      <c r="M59" s="62"/>
+      <c r="N59" s="59"/>
+      <c r="O59" s="46"/>
+      <c r="P59" s="47"/>
       <c r="AA59"/>
       <c r="AB59"/>
       <c r="AC59"/>
@@ -4117,15 +4303,15 @@
       <c r="AH59"/>
       <c r="AI59"/>
     </row>
-    <row r="60" spans="5:35" x14ac:dyDescent="0.3">
-      <c r="K60" s="26" t="s">
+    <row r="60" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="K60" s="60" t="s">
         <v>167</v>
       </c>
-      <c r="L60" s="27"/>
-      <c r="M60" s="28"/>
-      <c r="N60" s="41"/>
-      <c r="O60" s="27"/>
-      <c r="P60" s="32"/>
+      <c r="L60" s="61"/>
+      <c r="M60" s="62"/>
+      <c r="N60" s="59"/>
+      <c r="O60" s="46"/>
+      <c r="P60" s="47"/>
       <c r="AA60"/>
       <c r="AB60"/>
       <c r="AC60"/>
@@ -4136,15 +4322,15 @@
       <c r="AH60"/>
       <c r="AI60"/>
     </row>
-    <row r="61" spans="5:35" x14ac:dyDescent="0.3">
-      <c r="K61" s="26" t="s">
+    <row r="61" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="K61" s="60" t="s">
         <v>168</v>
       </c>
-      <c r="L61" s="27"/>
-      <c r="M61" s="28"/>
-      <c r="N61" s="41"/>
-      <c r="O61" s="27"/>
-      <c r="P61" s="32"/>
+      <c r="L61" s="61"/>
+      <c r="M61" s="62"/>
+      <c r="N61" s="59"/>
+      <c r="O61" s="46"/>
+      <c r="P61" s="47"/>
       <c r="AA61"/>
       <c r="AB61"/>
       <c r="AC61"/>
@@ -4155,15 +4341,15 @@
       <c r="AH61"/>
       <c r="AI61"/>
     </row>
-    <row r="62" spans="5:35" x14ac:dyDescent="0.3">
-      <c r="K62" s="26" t="s">
+    <row r="62" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="K62" s="60" t="s">
         <v>169</v>
       </c>
-      <c r="L62" s="27"/>
-      <c r="M62" s="28"/>
-      <c r="N62" s="41"/>
-      <c r="O62" s="27"/>
-      <c r="P62" s="32"/>
+      <c r="L62" s="61"/>
+      <c r="M62" s="62"/>
+      <c r="N62" s="59"/>
+      <c r="O62" s="46"/>
+      <c r="P62" s="47"/>
       <c r="AA62"/>
       <c r="AB62"/>
       <c r="AC62"/>
@@ -4174,15 +4360,15 @@
       <c r="AH62"/>
       <c r="AI62"/>
     </row>
-    <row r="63" spans="5:35" x14ac:dyDescent="0.3">
-      <c r="K63" s="26" t="s">
+    <row r="63" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="K63" s="60" t="s">
         <v>170</v>
       </c>
-      <c r="L63" s="27"/>
-      <c r="M63" s="28"/>
-      <c r="N63" s="41"/>
-      <c r="O63" s="27"/>
-      <c r="P63" s="32"/>
+      <c r="L63" s="61"/>
+      <c r="M63" s="62"/>
+      <c r="N63" s="59"/>
+      <c r="O63" s="46"/>
+      <c r="P63" s="47"/>
       <c r="AA63"/>
       <c r="AB63"/>
       <c r="AC63"/>
@@ -4193,15 +4379,15 @@
       <c r="AH63"/>
       <c r="AI63"/>
     </row>
-    <row r="64" spans="5:35" x14ac:dyDescent="0.3">
-      <c r="K64" s="26" t="s">
+    <row r="64" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="K64" s="60" t="s">
         <v>171</v>
       </c>
-      <c r="L64" s="27"/>
-      <c r="M64" s="28"/>
-      <c r="N64" s="41"/>
-      <c r="O64" s="27"/>
-      <c r="P64" s="32"/>
+      <c r="L64" s="61"/>
+      <c r="M64" s="62"/>
+      <c r="N64" s="59"/>
+      <c r="O64" s="46"/>
+      <c r="P64" s="47"/>
       <c r="AA64"/>
       <c r="AB64"/>
       <c r="AC64"/>
@@ -4213,14 +4399,14 @@
       <c r="AI64"/>
     </row>
     <row r="65" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K65" s="26" t="s">
+      <c r="K65" s="60" t="s">
         <v>172</v>
       </c>
-      <c r="L65" s="27"/>
-      <c r="M65" s="28"/>
-      <c r="N65" s="41"/>
-      <c r="O65" s="27"/>
-      <c r="P65" s="32"/>
+      <c r="L65" s="61"/>
+      <c r="M65" s="62"/>
+      <c r="N65" s="59"/>
+      <c r="O65" s="46"/>
+      <c r="P65" s="47"/>
       <c r="AA65"/>
       <c r="AB65"/>
       <c r="AC65"/>
@@ -4232,14 +4418,14 @@
       <c r="AI65"/>
     </row>
     <row r="66" spans="11:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K66" s="29" t="s">
+      <c r="K66" s="63" t="s">
         <v>173</v>
       </c>
-      <c r="L66" s="30"/>
-      <c r="M66" s="31"/>
-      <c r="N66" s="42"/>
-      <c r="O66" s="30"/>
-      <c r="P66" s="33"/>
+      <c r="L66" s="64"/>
+      <c r="M66" s="65"/>
+      <c r="N66" s="58"/>
+      <c r="O66" s="48"/>
+      <c r="P66" s="49"/>
       <c r="AA66"/>
       <c r="AB66"/>
       <c r="AC66"/>
@@ -4251,14 +4437,14 @@
       <c r="AI66"/>
     </row>
     <row r="67" spans="11:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K67" s="34" t="s">
+      <c r="K67" s="50" t="s">
         <v>219</v>
       </c>
-      <c r="L67" s="35"/>
-      <c r="M67" s="35"/>
-      <c r="N67" s="35"/>
-      <c r="O67" s="35"/>
-      <c r="P67" s="36"/>
+      <c r="L67" s="51"/>
+      <c r="M67" s="51"/>
+      <c r="N67" s="51"/>
+      <c r="O67" s="51"/>
+      <c r="P67" s="52"/>
       <c r="AA67"/>
       <c r="AB67"/>
       <c r="AC67"/>
@@ -4270,14 +4456,14 @@
       <c r="AI67"/>
     </row>
     <row r="68" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K68" s="37" t="s">
+      <c r="K68" s="53" t="s">
         <v>220</v>
       </c>
-      <c r="L68" s="38"/>
-      <c r="M68" s="39"/>
-      <c r="N68" s="38"/>
-      <c r="O68" s="38"/>
-      <c r="P68" s="40"/>
+      <c r="L68" s="54"/>
+      <c r="M68" s="55"/>
+      <c r="N68" s="56"/>
+      <c r="O68" s="56"/>
+      <c r="P68" s="57"/>
       <c r="AA68"/>
       <c r="AB68"/>
       <c r="AC68"/>
@@ -4289,14 +4475,14 @@
       <c r="AI68"/>
     </row>
     <row r="69" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K69" s="26" t="s">
+      <c r="K69" s="40" t="s">
         <v>221</v>
       </c>
-      <c r="L69" s="27"/>
-      <c r="M69" s="28"/>
-      <c r="N69" s="27"/>
-      <c r="O69" s="27"/>
-      <c r="P69" s="32"/>
+      <c r="L69" s="41"/>
+      <c r="M69" s="42"/>
+      <c r="N69" s="46"/>
+      <c r="O69" s="46"/>
+      <c r="P69" s="47"/>
       <c r="AA69"/>
       <c r="AB69"/>
       <c r="AC69"/>
@@ -4308,14 +4494,14 @@
       <c r="AI69"/>
     </row>
     <row r="70" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K70" s="26" t="s">
+      <c r="K70" s="40" t="s">
         <v>222</v>
       </c>
-      <c r="L70" s="27"/>
-      <c r="M70" s="28"/>
-      <c r="N70" s="27"/>
-      <c r="O70" s="27"/>
-      <c r="P70" s="32"/>
+      <c r="L70" s="41"/>
+      <c r="M70" s="42"/>
+      <c r="N70" s="46"/>
+      <c r="O70" s="46"/>
+      <c r="P70" s="47"/>
       <c r="AA70"/>
       <c r="AB70"/>
       <c r="AC70"/>
@@ -4327,14 +4513,14 @@
       <c r="AI70"/>
     </row>
     <row r="71" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K71" s="26" t="s">
+      <c r="K71" s="40" t="s">
         <v>223</v>
       </c>
-      <c r="L71" s="27"/>
-      <c r="M71" s="28"/>
-      <c r="N71" s="27"/>
-      <c r="O71" s="27"/>
-      <c r="P71" s="32"/>
+      <c r="L71" s="41"/>
+      <c r="M71" s="42"/>
+      <c r="N71" s="46"/>
+      <c r="O71" s="46"/>
+      <c r="P71" s="47"/>
       <c r="AA71"/>
       <c r="AB71"/>
       <c r="AC71"/>
@@ -4346,14 +4532,14 @@
       <c r="AI71"/>
     </row>
     <row r="72" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K72" s="26" t="s">
+      <c r="K72" s="40" t="s">
         <v>224</v>
       </c>
-      <c r="L72" s="27"/>
-      <c r="M72" s="28"/>
-      <c r="N72" s="27"/>
-      <c r="O72" s="27"/>
-      <c r="P72" s="32"/>
+      <c r="L72" s="41"/>
+      <c r="M72" s="42"/>
+      <c r="N72" s="46"/>
+      <c r="O72" s="46"/>
+      <c r="P72" s="47"/>
       <c r="AA72"/>
       <c r="AB72"/>
       <c r="AC72"/>
@@ -4365,14 +4551,14 @@
       <c r="AI72"/>
     </row>
     <row r="73" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K73" s="26" t="s">
+      <c r="K73" s="40" t="s">
         <v>225</v>
       </c>
-      <c r="L73" s="27"/>
-      <c r="M73" s="28"/>
-      <c r="N73" s="27"/>
-      <c r="O73" s="27"/>
-      <c r="P73" s="32"/>
+      <c r="L73" s="41"/>
+      <c r="M73" s="42"/>
+      <c r="N73" s="46"/>
+      <c r="O73" s="46"/>
+      <c r="P73" s="47"/>
       <c r="AA73"/>
       <c r="AB73"/>
       <c r="AC73"/>
@@ -4384,14 +4570,14 @@
       <c r="AI73"/>
     </row>
     <row r="74" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K74" s="26" t="s">
+      <c r="K74" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="L74" s="27"/>
-      <c r="M74" s="28"/>
-      <c r="N74" s="27"/>
-      <c r="O74" s="27"/>
-      <c r="P74" s="32"/>
+      <c r="L74" s="41"/>
+      <c r="M74" s="42"/>
+      <c r="N74" s="46"/>
+      <c r="O74" s="46"/>
+      <c r="P74" s="47"/>
       <c r="AA74"/>
       <c r="AB74"/>
       <c r="AC74"/>
@@ -4403,14 +4589,14 @@
       <c r="AI74"/>
     </row>
     <row r="75" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K75" s="26" t="s">
+      <c r="K75" s="40" t="s">
         <v>227</v>
       </c>
-      <c r="L75" s="27"/>
-      <c r="M75" s="28"/>
-      <c r="N75" s="27"/>
-      <c r="O75" s="27"/>
-      <c r="P75" s="32"/>
+      <c r="L75" s="41"/>
+      <c r="M75" s="42"/>
+      <c r="N75" s="46"/>
+      <c r="O75" s="46"/>
+      <c r="P75" s="47"/>
       <c r="AA75"/>
       <c r="AB75"/>
       <c r="AC75"/>
@@ -4422,14 +4608,14 @@
       <c r="AI75"/>
     </row>
     <row r="76" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K76" s="26" t="s">
+      <c r="K76" s="40" t="s">
         <v>228</v>
       </c>
-      <c r="L76" s="27"/>
-      <c r="M76" s="28"/>
-      <c r="N76" s="27"/>
-      <c r="O76" s="27"/>
-      <c r="P76" s="32"/>
+      <c r="L76" s="41"/>
+      <c r="M76" s="42"/>
+      <c r="N76" s="46"/>
+      <c r="O76" s="46"/>
+      <c r="P76" s="47"/>
       <c r="AA76"/>
       <c r="AB76"/>
       <c r="AC76"/>
@@ -4441,14 +4627,14 @@
       <c r="AI76"/>
     </row>
     <row r="77" spans="11:35" x14ac:dyDescent="0.3">
-      <c r="K77" s="26" t="s">
+      <c r="K77" s="40" t="s">
         <v>229</v>
       </c>
-      <c r="L77" s="27"/>
-      <c r="M77" s="28"/>
-      <c r="N77" s="27"/>
-      <c r="O77" s="27"/>
-      <c r="P77" s="32"/>
+      <c r="L77" s="41"/>
+      <c r="M77" s="42"/>
+      <c r="N77" s="46"/>
+      <c r="O77" s="46"/>
+      <c r="P77" s="47"/>
       <c r="AA77"/>
       <c r="AB77"/>
       <c r="AC77"/>
@@ -4460,14 +4646,14 @@
       <c r="AI77"/>
     </row>
     <row r="78" spans="11:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K78" s="29" t="s">
+      <c r="K78" s="43" t="s">
         <v>230</v>
       </c>
-      <c r="L78" s="30"/>
-      <c r="M78" s="31"/>
-      <c r="N78" s="30"/>
-      <c r="O78" s="30"/>
-      <c r="P78" s="33"/>
+      <c r="L78" s="44"/>
+      <c r="M78" s="45"/>
+      <c r="N78" s="48"/>
+      <c r="O78" s="48"/>
+      <c r="P78" s="49"/>
       <c r="AA78"/>
       <c r="AB78"/>
       <c r="AC78"/>

</xml_diff>